<commit_message>
final version in master
</commit_message>
<xml_diff>
--- a/HighRiskInvestment.xlsx
+++ b/HighRiskInvestment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3585" windowWidth="14805" windowHeight="4530" tabRatio="771" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="3585" windowWidth="14805" windowHeight="4530" tabRatio="771" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ESPP" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </externalReferences>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -8834,6 +8834,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8843,17 +8846,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8868,93 +8868,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="52" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="52" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="54" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="54" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8978,6 +8891,93 @@
     <xf numFmtId="0" fontId="54" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="54" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="54" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="52" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="52" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -8993,12 +8993,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="19" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9019,18 +9013,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9055,6 +9037,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12346,7 +12346,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -12437,7 +12437,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -12833,11 +12833,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" customHeight="1">
-      <c r="A1" s="397" t="s">
+      <c r="A1" s="396" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="397"/>
-      <c r="C1" s="397"/>
+      <c r="B1" s="396"/>
+      <c r="C1" s="396"/>
       <c r="D1" s="110">
         <f>SUM(G10:G88)-SUM(L10:L88)</f>
         <v>268</v>
@@ -12850,11 +12850,11 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A2" s="398" t="s">
+      <c r="A2" s="397" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="398"/>
-      <c r="C2" s="398"/>
+      <c r="B2" s="397"/>
+      <c r="C2" s="397"/>
       <c r="D2" s="111">
         <v>29.75</v>
       </c>
@@ -12869,11 +12869,11 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A3" s="398" t="s">
+      <c r="A3" s="397" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="398"/>
-      <c r="C3" s="398"/>
+      <c r="B3" s="397"/>
+      <c r="C3" s="397"/>
       <c r="D3" s="111">
         <f>D1*0.85</f>
         <v>227.79999999999998</v>
@@ -12889,11 +12889,11 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A4" s="398" t="s">
+      <c r="A4" s="397" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="398"/>
-      <c r="C4" s="398"/>
+      <c r="B4" s="397"/>
+      <c r="C4" s="397"/>
       <c r="D4" s="112">
         <f>([1]Sheet2!B64)/100</f>
         <v>6.1073000000000004</v>
@@ -12903,11 +12903,11 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1">
-      <c r="A5" s="396" t="s">
+      <c r="A5" s="392" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="396"/>
-      <c r="C5" s="396"/>
+      <c r="B5" s="392"/>
+      <c r="C5" s="392"/>
       <c r="D5" s="113">
         <f>SUM(D10:D88)+SUM(H10:H88)</f>
         <v>76568.666499999992</v>
@@ -12917,11 +12917,11 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A6" s="396" t="s">
+      <c r="A6" s="392" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="396"/>
-      <c r="C6" s="396"/>
+      <c r="B6" s="392"/>
+      <c r="C6" s="392"/>
       <c r="D6" s="114">
         <f>SUM(Q10:Q88)</f>
         <v>48178.589949999994</v>
@@ -12935,11 +12935,11 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19.5" customHeight="1">
-      <c r="A7" s="396" t="s">
+      <c r="A7" s="392" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="396"/>
-      <c r="C7" s="396"/>
+      <c r="B7" s="392"/>
+      <c r="C7" s="392"/>
       <c r="D7" s="116">
         <f>D6-D5</f>
         <v>-28390.076549999998</v>
@@ -13018,38 +13018,38 @@
       <c r="B10" s="109">
         <v>0</v>
       </c>
-      <c r="C10" s="392">
+      <c r="C10" s="393">
         <v>68.97</v>
       </c>
-      <c r="D10" s="393">
+      <c r="D10" s="394">
         <f>IF(B15&gt;0,SUM(B10:B15)-C10,0)</f>
         <v>10580.78</v>
       </c>
-      <c r="E10" s="392">
+      <c r="E10" s="393">
         <v>6.2854999999999999</v>
       </c>
-      <c r="F10" s="392">
+      <c r="F10" s="393">
         <v>25.3</v>
       </c>
-      <c r="G10" s="394">
+      <c r="G10" s="395">
         <v>79</v>
       </c>
       <c r="H10" s="120">
         <f t="shared" ref="H10:H15" si="0">R16*0.2</f>
         <v>62.814</v>
       </c>
-      <c r="I10" s="395">
+      <c r="I10" s="398">
         <f>IF($K$28&gt;F10,G10*($K$28-F10)*0.2,0)</f>
         <v>70.309999999999988</v>
       </c>
-      <c r="J10" s="395"/>
-      <c r="K10" s="395"/>
-      <c r="L10" s="395"/>
-      <c r="M10" s="395"/>
-      <c r="N10" s="395"/>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
-      <c r="Q10" s="395"/>
+      <c r="J10" s="398"/>
+      <c r="K10" s="398"/>
+      <c r="L10" s="398"/>
+      <c r="M10" s="398"/>
+      <c r="N10" s="398"/>
+      <c r="O10" s="398"/>
+      <c r="P10" s="398"/>
+      <c r="Q10" s="398"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1">
@@ -13058,26 +13058,26 @@
       <c r="B11" s="109">
         <v>3400.95</v>
       </c>
-      <c r="C11" s="392">
+      <c r="C11" s="393">
         <v>3400.95</v>
       </c>
-      <c r="D11" s="393"/>
-      <c r="E11" s="392"/>
-      <c r="F11" s="392"/>
-      <c r="G11" s="394"/>
+      <c r="D11" s="394"/>
+      <c r="E11" s="393"/>
+      <c r="F11" s="393"/>
+      <c r="G11" s="395"/>
       <c r="H11" s="120">
         <f t="shared" si="0"/>
         <v>62.814</v>
       </c>
-      <c r="I11" s="395"/>
-      <c r="J11" s="395"/>
-      <c r="K11" s="395"/>
-      <c r="L11" s="395"/>
-      <c r="M11" s="395"/>
-      <c r="N11" s="395"/>
-      <c r="O11" s="395"/>
-      <c r="P11" s="395"/>
-      <c r="Q11" s="395"/>
+      <c r="I11" s="398"/>
+      <c r="J11" s="398"/>
+      <c r="K11" s="398"/>
+      <c r="L11" s="398"/>
+      <c r="M11" s="398"/>
+      <c r="N11" s="398"/>
+      <c r="O11" s="398"/>
+      <c r="P11" s="398"/>
+      <c r="Q11" s="398"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="1">
@@ -13086,26 +13086,26 @@
       <c r="B12" s="109">
         <v>1706.25</v>
       </c>
-      <c r="C12" s="392">
+      <c r="C12" s="393">
         <v>1706.25</v>
       </c>
-      <c r="D12" s="393"/>
-      <c r="E12" s="392"/>
-      <c r="F12" s="392"/>
-      <c r="G12" s="394"/>
+      <c r="D12" s="394"/>
+      <c r="E12" s="393"/>
+      <c r="F12" s="393"/>
+      <c r="G12" s="395"/>
       <c r="H12" s="120">
         <f t="shared" si="0"/>
         <v>62.814</v>
       </c>
-      <c r="I12" s="395"/>
-      <c r="J12" s="395"/>
-      <c r="K12" s="395"/>
-      <c r="L12" s="395"/>
-      <c r="M12" s="395"/>
-      <c r="N12" s="395"/>
-      <c r="O12" s="395"/>
-      <c r="P12" s="395"/>
-      <c r="Q12" s="395"/>
+      <c r="I12" s="398"/>
+      <c r="J12" s="398"/>
+      <c r="K12" s="398"/>
+      <c r="L12" s="398"/>
+      <c r="M12" s="398"/>
+      <c r="N12" s="398"/>
+      <c r="O12" s="398"/>
+      <c r="P12" s="398"/>
+      <c r="Q12" s="398"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="1">
@@ -13114,26 +13114,26 @@
       <c r="B13" s="109">
         <v>1706.25</v>
       </c>
-      <c r="C13" s="392">
+      <c r="C13" s="393">
         <v>1706.25</v>
       </c>
-      <c r="D13" s="393"/>
-      <c r="E13" s="392"/>
-      <c r="F13" s="392"/>
-      <c r="G13" s="394"/>
+      <c r="D13" s="394"/>
+      <c r="E13" s="393"/>
+      <c r="F13" s="393"/>
+      <c r="G13" s="395"/>
       <c r="H13" s="120">
         <f t="shared" si="0"/>
         <v>62.814</v>
       </c>
-      <c r="I13" s="395"/>
-      <c r="J13" s="395"/>
-      <c r="K13" s="395"/>
-      <c r="L13" s="395"/>
-      <c r="M13" s="395"/>
-      <c r="N13" s="395"/>
-      <c r="O13" s="395"/>
-      <c r="P13" s="395"/>
-      <c r="Q13" s="395"/>
+      <c r="I13" s="398"/>
+      <c r="J13" s="398"/>
+      <c r="K13" s="398"/>
+      <c r="L13" s="398"/>
+      <c r="M13" s="398"/>
+      <c r="N13" s="398"/>
+      <c r="O13" s="398"/>
+      <c r="P13" s="398"/>
+      <c r="Q13" s="398"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1">
@@ -13142,26 +13142,26 @@
       <c r="B14" s="109">
         <v>1918.15</v>
       </c>
-      <c r="C14" s="392">
+      <c r="C14" s="393">
         <v>1918.15</v>
       </c>
-      <c r="D14" s="393"/>
-      <c r="E14" s="392"/>
-      <c r="F14" s="392"/>
-      <c r="G14" s="394"/>
+      <c r="D14" s="394"/>
+      <c r="E14" s="393"/>
+      <c r="F14" s="393"/>
+      <c r="G14" s="395"/>
       <c r="H14" s="120">
         <f t="shared" si="0"/>
         <v>62.814</v>
       </c>
-      <c r="I14" s="395"/>
-      <c r="J14" s="395"/>
-      <c r="K14" s="395"/>
-      <c r="L14" s="395"/>
-      <c r="M14" s="395"/>
-      <c r="N14" s="395"/>
-      <c r="O14" s="395"/>
-      <c r="P14" s="395"/>
-      <c r="Q14" s="395"/>
+      <c r="I14" s="398"/>
+      <c r="J14" s="398"/>
+      <c r="K14" s="398"/>
+      <c r="L14" s="398"/>
+      <c r="M14" s="398"/>
+      <c r="N14" s="398"/>
+      <c r="O14" s="398"/>
+      <c r="P14" s="398"/>
+      <c r="Q14" s="398"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1">
@@ -13170,26 +13170,26 @@
       <c r="B15" s="109">
         <v>1918.15</v>
       </c>
-      <c r="C15" s="392">
+      <c r="C15" s="393">
         <v>1918.15</v>
       </c>
-      <c r="D15" s="393"/>
-      <c r="E15" s="392"/>
-      <c r="F15" s="392"/>
-      <c r="G15" s="394"/>
+      <c r="D15" s="394"/>
+      <c r="E15" s="393"/>
+      <c r="F15" s="393"/>
+      <c r="G15" s="395"/>
       <c r="H15" s="120">
         <f t="shared" si="0"/>
         <v>62.814</v>
       </c>
-      <c r="I15" s="395"/>
-      <c r="J15" s="395"/>
-      <c r="K15" s="395"/>
-      <c r="L15" s="395"/>
-      <c r="M15" s="395"/>
-      <c r="N15" s="395"/>
-      <c r="O15" s="395"/>
-      <c r="P15" s="395"/>
-      <c r="Q15" s="395"/>
+      <c r="I15" s="398"/>
+      <c r="J15" s="398"/>
+      <c r="K15" s="398"/>
+      <c r="L15" s="398"/>
+      <c r="M15" s="398"/>
+      <c r="N15" s="398"/>
+      <c r="O15" s="398"/>
+      <c r="P15" s="398"/>
+      <c r="Q15" s="398"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="1">
@@ -13198,38 +13198,38 @@
       <c r="B16" s="109">
         <v>1693.15</v>
       </c>
-      <c r="C16" s="392">
+      <c r="C16" s="393">
         <v>48.24</v>
       </c>
-      <c r="D16" s="393">
+      <c r="D16" s="394">
         <f>IF(B21&gt;0,SUM(B16:B21)-C16,0)</f>
         <v>11196.460000000001</v>
       </c>
-      <c r="E16" s="392">
+      <c r="E16" s="393">
         <v>6.1787000000000001</v>
       </c>
-      <c r="F16" s="392">
+      <c r="F16" s="393">
         <v>23.62</v>
       </c>
-      <c r="G16" s="394">
+      <c r="G16" s="395">
         <v>90</v>
       </c>
       <c r="H16" s="120">
         <f>R22*0.25</f>
         <v>81.435000000000002</v>
       </c>
-      <c r="I16" s="395">
+      <c r="I16" s="398">
         <f>IF($K$28&gt;F16,G16*($K$28-F16)*0.2,0)</f>
         <v>110.33999999999999</v>
       </c>
-      <c r="J16" s="395"/>
-      <c r="K16" s="395"/>
-      <c r="L16" s="395"/>
-      <c r="M16" s="395"/>
-      <c r="N16" s="395"/>
-      <c r="O16" s="395"/>
-      <c r="P16" s="395"/>
-      <c r="Q16" s="395"/>
+      <c r="J16" s="398"/>
+      <c r="K16" s="398"/>
+      <c r="L16" s="398"/>
+      <c r="M16" s="398"/>
+      <c r="N16" s="398"/>
+      <c r="O16" s="398"/>
+      <c r="P16" s="398"/>
+      <c r="Q16" s="398"/>
       <c r="R16" s="109">
         <v>314.07</v>
       </c>
@@ -13241,24 +13241,24 @@
       <c r="B17" s="121">
         <v>1719.35</v>
       </c>
-      <c r="C17" s="392"/>
-      <c r="D17" s="393"/>
-      <c r="E17" s="392"/>
-      <c r="F17" s="392"/>
-      <c r="G17" s="394"/>
+      <c r="C17" s="393"/>
+      <c r="D17" s="394"/>
+      <c r="E17" s="393"/>
+      <c r="F17" s="393"/>
+      <c r="G17" s="395"/>
       <c r="H17" s="120">
         <f t="shared" ref="H17:H80" si="1">R23*0.25</f>
         <v>67.862499999999997</v>
       </c>
-      <c r="I17" s="395"/>
-      <c r="J17" s="395"/>
-      <c r="K17" s="395"/>
-      <c r="L17" s="395"/>
-      <c r="M17" s="395"/>
-      <c r="N17" s="395"/>
-      <c r="O17" s="395"/>
-      <c r="P17" s="395"/>
-      <c r="Q17" s="395"/>
+      <c r="I17" s="398"/>
+      <c r="J17" s="398"/>
+      <c r="K17" s="398"/>
+      <c r="L17" s="398"/>
+      <c r="M17" s="398"/>
+      <c r="N17" s="398"/>
+      <c r="O17" s="398"/>
+      <c r="P17" s="398"/>
+      <c r="Q17" s="398"/>
       <c r="R17" s="109">
         <f>R16</f>
         <v>314.07</v>
@@ -13271,24 +13271,24 @@
       <c r="B18" s="121">
         <v>1719.35</v>
       </c>
-      <c r="C18" s="392"/>
-      <c r="D18" s="393"/>
-      <c r="E18" s="392"/>
-      <c r="F18" s="392"/>
-      <c r="G18" s="394"/>
+      <c r="C18" s="393"/>
+      <c r="D18" s="394"/>
+      <c r="E18" s="393"/>
+      <c r="F18" s="393"/>
+      <c r="G18" s="395"/>
       <c r="H18" s="120">
         <f t="shared" si="1"/>
         <v>67.862499999999997</v>
       </c>
-      <c r="I18" s="395"/>
-      <c r="J18" s="395"/>
-      <c r="K18" s="395"/>
-      <c r="L18" s="395"/>
-      <c r="M18" s="395"/>
-      <c r="N18" s="395"/>
-      <c r="O18" s="395"/>
-      <c r="P18" s="395"/>
-      <c r="Q18" s="395"/>
+      <c r="I18" s="398"/>
+      <c r="J18" s="398"/>
+      <c r="K18" s="398"/>
+      <c r="L18" s="398"/>
+      <c r="M18" s="398"/>
+      <c r="N18" s="398"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
+      <c r="Q18" s="398"/>
       <c r="R18" s="109">
         <f t="shared" ref="R18:R32" si="2">R17</f>
         <v>314.07</v>
@@ -13301,24 +13301,24 @@
       <c r="B19" s="121">
         <v>2196.35</v>
       </c>
-      <c r="C19" s="392"/>
-      <c r="D19" s="393"/>
-      <c r="E19" s="392"/>
-      <c r="F19" s="392"/>
-      <c r="G19" s="394"/>
+      <c r="C19" s="393"/>
+      <c r="D19" s="394"/>
+      <c r="E19" s="393"/>
+      <c r="F19" s="393"/>
+      <c r="G19" s="395"/>
       <c r="H19" s="120">
         <f t="shared" si="1"/>
         <v>67.862499999999997</v>
       </c>
-      <c r="I19" s="395"/>
-      <c r="J19" s="395"/>
-      <c r="K19" s="395"/>
-      <c r="L19" s="395"/>
-      <c r="M19" s="395"/>
-      <c r="N19" s="395"/>
-      <c r="O19" s="395"/>
-      <c r="P19" s="395"/>
-      <c r="Q19" s="395"/>
+      <c r="I19" s="398"/>
+      <c r="J19" s="398"/>
+      <c r="K19" s="398"/>
+      <c r="L19" s="398"/>
+      <c r="M19" s="398"/>
+      <c r="N19" s="398"/>
+      <c r="O19" s="398"/>
+      <c r="P19" s="398"/>
+      <c r="Q19" s="398"/>
       <c r="R19" s="109">
         <f t="shared" si="2"/>
         <v>314.07</v>
@@ -13331,24 +13331,24 @@
       <c r="B20" s="121">
         <v>1958.25</v>
       </c>
-      <c r="C20" s="392"/>
-      <c r="D20" s="393"/>
-      <c r="E20" s="392"/>
-      <c r="F20" s="392"/>
-      <c r="G20" s="394"/>
+      <c r="C20" s="393"/>
+      <c r="D20" s="394"/>
+      <c r="E20" s="393"/>
+      <c r="F20" s="393"/>
+      <c r="G20" s="395"/>
       <c r="H20" s="120">
         <f t="shared" si="1"/>
         <v>67.862499999999997</v>
       </c>
-      <c r="I20" s="395"/>
-      <c r="J20" s="395"/>
-      <c r="K20" s="395"/>
-      <c r="L20" s="395"/>
-      <c r="M20" s="395"/>
-      <c r="N20" s="395"/>
-      <c r="O20" s="395"/>
-      <c r="P20" s="395"/>
-      <c r="Q20" s="395"/>
+      <c r="I20" s="398"/>
+      <c r="J20" s="398"/>
+      <c r="K20" s="398"/>
+      <c r="L20" s="398"/>
+      <c r="M20" s="398"/>
+      <c r="N20" s="398"/>
+      <c r="O20" s="398"/>
+      <c r="P20" s="398"/>
+      <c r="Q20" s="398"/>
       <c r="R20" s="109">
         <f t="shared" si="2"/>
         <v>314.07</v>
@@ -13361,24 +13361,24 @@
       <c r="B21" s="121">
         <v>1958.25</v>
       </c>
-      <c r="C21" s="392"/>
-      <c r="D21" s="393"/>
-      <c r="E21" s="392"/>
-      <c r="F21" s="392"/>
-      <c r="G21" s="394"/>
+      <c r="C21" s="393"/>
+      <c r="D21" s="394"/>
+      <c r="E21" s="393"/>
+      <c r="F21" s="393"/>
+      <c r="G21" s="395"/>
       <c r="H21" s="120">
         <f t="shared" si="1"/>
         <v>67.862499999999997</v>
       </c>
-      <c r="I21" s="395"/>
-      <c r="J21" s="395"/>
-      <c r="K21" s="395"/>
-      <c r="L21" s="395"/>
-      <c r="M21" s="395"/>
-      <c r="N21" s="395"/>
-      <c r="O21" s="395"/>
-      <c r="P21" s="395"/>
-      <c r="Q21" s="395"/>
+      <c r="I21" s="398"/>
+      <c r="J21" s="398"/>
+      <c r="K21" s="398"/>
+      <c r="L21" s="398"/>
+      <c r="M21" s="398"/>
+      <c r="N21" s="398"/>
+      <c r="O21" s="398"/>
+      <c r="P21" s="398"/>
+      <c r="Q21" s="398"/>
       <c r="R21" s="109">
         <f t="shared" si="2"/>
         <v>314.07</v>
@@ -13391,38 +13391,38 @@
       <c r="B22" s="121">
         <v>1958.23</v>
       </c>
-      <c r="C22" s="392">
+      <c r="C22" s="393">
         <v>34.549999999999997</v>
       </c>
-      <c r="D22" s="393">
+      <c r="D22" s="394">
         <f>IF(B27&gt;0,SUM(B22:B27)-C22,0)</f>
         <v>11771.410000000002</v>
       </c>
-      <c r="E22" s="392">
+      <c r="E22" s="393">
         <v>6.1050000000000004</v>
       </c>
-      <c r="F22" s="392">
+      <c r="F22" s="393">
         <v>24.24</v>
       </c>
-      <c r="G22" s="394">
+      <c r="G22" s="395">
         <v>109</v>
       </c>
       <c r="H22" s="120">
         <f>R28*0.25</f>
         <v>67.862499999999997</v>
       </c>
-      <c r="I22" s="395">
+      <c r="I22" s="398">
         <f>IF($K$28&gt;F22,G22*($K$28-F22)*0.2,0)</f>
         <v>120.11800000000004</v>
       </c>
-      <c r="J22" s="395"/>
-      <c r="K22" s="395"/>
-      <c r="L22" s="395"/>
-      <c r="M22" s="395"/>
-      <c r="N22" s="395"/>
-      <c r="O22" s="395"/>
-      <c r="P22" s="395"/>
-      <c r="Q22" s="395"/>
+      <c r="J22" s="398"/>
+      <c r="K22" s="398"/>
+      <c r="L22" s="398"/>
+      <c r="M22" s="398"/>
+      <c r="N22" s="398"/>
+      <c r="O22" s="398"/>
+      <c r="P22" s="398"/>
+      <c r="Q22" s="398"/>
       <c r="R22" s="109">
         <v>325.74</v>
       </c>
@@ -13434,24 +13434,24 @@
       <c r="B23" s="121">
         <v>1958.24</v>
       </c>
-      <c r="C23" s="392"/>
-      <c r="D23" s="393"/>
-      <c r="E23" s="392"/>
-      <c r="F23" s="392"/>
-      <c r="G23" s="394"/>
+      <c r="C23" s="393"/>
+      <c r="D23" s="394"/>
+      <c r="E23" s="393"/>
+      <c r="F23" s="393"/>
+      <c r="G23" s="395"/>
       <c r="H23" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I23" s="395"/>
-      <c r="J23" s="395"/>
-      <c r="K23" s="395"/>
-      <c r="L23" s="395"/>
-      <c r="M23" s="395"/>
-      <c r="N23" s="395"/>
-      <c r="O23" s="395"/>
-      <c r="P23" s="395"/>
-      <c r="Q23" s="395"/>
+      <c r="I23" s="398"/>
+      <c r="J23" s="398"/>
+      <c r="K23" s="398"/>
+      <c r="L23" s="398"/>
+      <c r="M23" s="398"/>
+      <c r="N23" s="398"/>
+      <c r="O23" s="398"/>
+      <c r="P23" s="398"/>
+      <c r="Q23" s="398"/>
       <c r="R23" s="109">
         <v>271.45</v>
       </c>
@@ -13463,24 +13463,24 @@
       <c r="B24" s="121">
         <v>1958.25</v>
       </c>
-      <c r="C24" s="392"/>
-      <c r="D24" s="393"/>
-      <c r="E24" s="392"/>
-      <c r="F24" s="392"/>
-      <c r="G24" s="394"/>
+      <c r="C24" s="393"/>
+      <c r="D24" s="394"/>
+      <c r="E24" s="393"/>
+      <c r="F24" s="393"/>
+      <c r="G24" s="395"/>
       <c r="H24" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I24" s="395"/>
-      <c r="J24" s="395"/>
-      <c r="K24" s="395"/>
-      <c r="L24" s="395"/>
-      <c r="M24" s="395"/>
-      <c r="N24" s="395"/>
-      <c r="O24" s="395"/>
-      <c r="P24" s="395"/>
-      <c r="Q24" s="395"/>
+      <c r="I24" s="398"/>
+      <c r="J24" s="398"/>
+      <c r="K24" s="398"/>
+      <c r="L24" s="398"/>
+      <c r="M24" s="398"/>
+      <c r="N24" s="398"/>
+      <c r="O24" s="398"/>
+      <c r="P24" s="398"/>
+      <c r="Q24" s="398"/>
       <c r="R24" s="109">
         <f t="shared" si="2"/>
         <v>271.45</v>
@@ -13493,24 +13493,24 @@
       <c r="B25" s="121">
         <v>1958.26</v>
       </c>
-      <c r="C25" s="392"/>
-      <c r="D25" s="393"/>
-      <c r="E25" s="392"/>
-      <c r="F25" s="392"/>
-      <c r="G25" s="394"/>
+      <c r="C25" s="393"/>
+      <c r="D25" s="394"/>
+      <c r="E25" s="393"/>
+      <c r="F25" s="393"/>
+      <c r="G25" s="395"/>
       <c r="H25" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I25" s="395"/>
-      <c r="J25" s="395"/>
-      <c r="K25" s="395"/>
-      <c r="L25" s="395"/>
-      <c r="M25" s="395"/>
-      <c r="N25" s="395"/>
-      <c r="O25" s="395"/>
-      <c r="P25" s="395"/>
-      <c r="Q25" s="395"/>
+      <c r="I25" s="398"/>
+      <c r="J25" s="398"/>
+      <c r="K25" s="398"/>
+      <c r="L25" s="398"/>
+      <c r="M25" s="398"/>
+      <c r="N25" s="398"/>
+      <c r="O25" s="398"/>
+      <c r="P25" s="398"/>
+      <c r="Q25" s="398"/>
       <c r="R25" s="109">
         <f t="shared" si="2"/>
         <v>271.45</v>
@@ -13523,24 +13523,24 @@
       <c r="B26" s="121">
         <v>2031.49</v>
       </c>
-      <c r="C26" s="392"/>
-      <c r="D26" s="393"/>
-      <c r="E26" s="392"/>
-      <c r="F26" s="392"/>
-      <c r="G26" s="394"/>
+      <c r="C26" s="393"/>
+      <c r="D26" s="394"/>
+      <c r="E26" s="393"/>
+      <c r="F26" s="393"/>
+      <c r="G26" s="395"/>
       <c r="H26" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I26" s="395"/>
-      <c r="J26" s="395"/>
-      <c r="K26" s="395"/>
-      <c r="L26" s="395"/>
-      <c r="M26" s="395"/>
-      <c r="N26" s="395"/>
-      <c r="O26" s="395"/>
-      <c r="P26" s="395"/>
-      <c r="Q26" s="395"/>
+      <c r="I26" s="398"/>
+      <c r="J26" s="398"/>
+      <c r="K26" s="398"/>
+      <c r="L26" s="398"/>
+      <c r="M26" s="398"/>
+      <c r="N26" s="398"/>
+      <c r="O26" s="398"/>
+      <c r="P26" s="398"/>
+      <c r="Q26" s="398"/>
       <c r="R26" s="109">
         <f t="shared" si="2"/>
         <v>271.45</v>
@@ -13553,24 +13553,24 @@
       <c r="B27" s="121">
         <v>1941.49</v>
       </c>
-      <c r="C27" s="392"/>
-      <c r="D27" s="393"/>
-      <c r="E27" s="392"/>
-      <c r="F27" s="392"/>
-      <c r="G27" s="394"/>
+      <c r="C27" s="393"/>
+      <c r="D27" s="394"/>
+      <c r="E27" s="393"/>
+      <c r="F27" s="393"/>
+      <c r="G27" s="395"/>
       <c r="H27" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I27" s="395"/>
-      <c r="J27" s="395"/>
-      <c r="K27" s="395"/>
-      <c r="L27" s="395"/>
-      <c r="M27" s="395"/>
-      <c r="N27" s="395"/>
-      <c r="O27" s="395"/>
-      <c r="P27" s="395"/>
-      <c r="Q27" s="395"/>
+      <c r="I27" s="398"/>
+      <c r="J27" s="398"/>
+      <c r="K27" s="398"/>
+      <c r="L27" s="398"/>
+      <c r="M27" s="398"/>
+      <c r="N27" s="398"/>
+      <c r="O27" s="398"/>
+      <c r="P27" s="398"/>
+      <c r="Q27" s="398"/>
       <c r="R27" s="109">
         <f t="shared" si="2"/>
         <v>271.45</v>
@@ -13583,54 +13583,54 @@
       <c r="B28" s="121">
         <v>1941.49</v>
       </c>
-      <c r="C28" s="392">
+      <c r="C28" s="393">
         <v>22.25</v>
       </c>
-      <c r="D28" s="393">
+      <c r="D28" s="394">
         <f>IF(G28&gt;0,SUM(B28:B34)-C28,0)</f>
         <v>14106.8</v>
       </c>
-      <c r="E28" s="392">
+      <c r="E28" s="393">
         <v>6.1675000000000004</v>
       </c>
-      <c r="F28" s="392">
+      <c r="F28" s="393">
         <v>29.3</v>
       </c>
-      <c r="G28" s="394">
+      <c r="G28" s="395">
         <v>79</v>
       </c>
       <c r="H28" s="120">
         <f t="shared" si="1"/>
         <v>100.08750000000001</v>
       </c>
-      <c r="I28" s="395">
+      <c r="I28" s="398">
         <f>IF($D$2&gt;F28,G28*($D$2-F28)*0.2,0)</f>
         <v>7.1099999999999888</v>
       </c>
-      <c r="J28" s="395">
+      <c r="J28" s="398">
         <f>SUM(I10:I27)</f>
         <v>300.76800000000003</v>
       </c>
-      <c r="K28" s="395">
+      <c r="K28" s="398">
         <v>29.75</v>
       </c>
-      <c r="L28" s="395">
+      <c r="L28" s="398">
         <v>278</v>
       </c>
-      <c r="M28" s="395">
+      <c r="M28" s="398">
         <f>IF(IF(L28*K28&lt;5000,L28*K28*0.006,L28*K28*0.005)&gt;25,IF(L28*K28&lt;5000,L28*K28*0.006,L28*K28*0.005),25)</f>
         <v>41.352499999999999</v>
       </c>
-      <c r="N28" s="395">
+      <c r="N28" s="398">
         <v>5.25</v>
       </c>
-      <c r="O28" s="395">
-        <v>0</v>
-      </c>
-      <c r="P28" s="395">
+      <c r="O28" s="398">
+        <v>0</v>
+      </c>
+      <c r="P28" s="398">
         <v>25</v>
       </c>
-      <c r="Q28" s="395">
+      <c r="Q28" s="398">
         <f>(K28*L28-J28-M28-N28-O28-P28)*S34</f>
         <v>48178.589949999994</v>
       </c>
@@ -13646,24 +13646,24 @@
       <c r="B29" s="121">
         <v>2445.75</v>
       </c>
-      <c r="C29" s="392"/>
-      <c r="D29" s="393"/>
-      <c r="E29" s="392"/>
-      <c r="F29" s="392"/>
-      <c r="G29" s="394"/>
+      <c r="C29" s="393"/>
+      <c r="D29" s="394"/>
+      <c r="E29" s="393"/>
+      <c r="F29" s="393"/>
+      <c r="G29" s="395"/>
       <c r="H29" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I29" s="395"/>
-      <c r="J29" s="395"/>
-      <c r="K29" s="395"/>
-      <c r="L29" s="395"/>
-      <c r="M29" s="395"/>
-      <c r="N29" s="395"/>
-      <c r="O29" s="395"/>
-      <c r="P29" s="395"/>
-      <c r="Q29" s="395"/>
+      <c r="I29" s="398"/>
+      <c r="J29" s="398"/>
+      <c r="K29" s="398"/>
+      <c r="L29" s="398"/>
+      <c r="M29" s="398"/>
+      <c r="N29" s="398"/>
+      <c r="O29" s="398"/>
+      <c r="P29" s="398"/>
+      <c r="Q29" s="398"/>
       <c r="R29" s="109">
         <v>400.35</v>
       </c>
@@ -13675,24 +13675,24 @@
       <c r="B30" s="121">
         <v>1917.03</v>
       </c>
-      <c r="C30" s="392"/>
-      <c r="D30" s="393"/>
-      <c r="E30" s="392"/>
-      <c r="F30" s="392"/>
-      <c r="G30" s="394"/>
+      <c r="C30" s="393"/>
+      <c r="D30" s="394"/>
+      <c r="E30" s="393"/>
+      <c r="F30" s="393"/>
+      <c r="G30" s="395"/>
       <c r="H30" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I30" s="395"/>
-      <c r="J30" s="395"/>
-      <c r="K30" s="395"/>
-      <c r="L30" s="395"/>
-      <c r="M30" s="395"/>
-      <c r="N30" s="395"/>
-      <c r="O30" s="395"/>
-      <c r="P30" s="395"/>
-      <c r="Q30" s="395"/>
+      <c r="I30" s="398"/>
+      <c r="J30" s="398"/>
+      <c r="K30" s="398"/>
+      <c r="L30" s="398"/>
+      <c r="M30" s="398"/>
+      <c r="N30" s="398"/>
+      <c r="O30" s="398"/>
+      <c r="P30" s="398"/>
+      <c r="Q30" s="398"/>
       <c r="R30" s="109">
         <f t="shared" si="2"/>
         <v>400.35</v>
@@ -13705,24 +13705,24 @@
       <c r="B31" s="121">
         <v>1827.02</v>
       </c>
-      <c r="C31" s="392"/>
-      <c r="D31" s="393"/>
-      <c r="E31" s="392"/>
-      <c r="F31" s="392"/>
-      <c r="G31" s="394"/>
+      <c r="C31" s="393"/>
+      <c r="D31" s="394"/>
+      <c r="E31" s="393"/>
+      <c r="F31" s="393"/>
+      <c r="G31" s="395"/>
       <c r="H31" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I31" s="395"/>
-      <c r="J31" s="395"/>
-      <c r="K31" s="395"/>
-      <c r="L31" s="395"/>
-      <c r="M31" s="395"/>
-      <c r="N31" s="395"/>
-      <c r="O31" s="395"/>
-      <c r="P31" s="395"/>
-      <c r="Q31" s="395"/>
+      <c r="I31" s="398"/>
+      <c r="J31" s="398"/>
+      <c r="K31" s="398"/>
+      <c r="L31" s="398"/>
+      <c r="M31" s="398"/>
+      <c r="N31" s="398"/>
+      <c r="O31" s="398"/>
+      <c r="P31" s="398"/>
+      <c r="Q31" s="398"/>
       <c r="R31" s="109">
         <f t="shared" si="2"/>
         <v>400.35</v>
@@ -13735,24 +13735,24 @@
       <c r="B32" s="121">
         <v>1958.22</v>
       </c>
-      <c r="C32" s="392"/>
-      <c r="D32" s="393"/>
-      <c r="E32" s="392"/>
-      <c r="F32" s="392"/>
-      <c r="G32" s="394"/>
+      <c r="C32" s="393"/>
+      <c r="D32" s="394"/>
+      <c r="E32" s="393"/>
+      <c r="F32" s="393"/>
+      <c r="G32" s="395"/>
       <c r="H32" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I32" s="395"/>
-      <c r="J32" s="395"/>
-      <c r="K32" s="395"/>
-      <c r="L32" s="395"/>
-      <c r="M32" s="395"/>
-      <c r="N32" s="395"/>
-      <c r="O32" s="395"/>
-      <c r="P32" s="395"/>
-      <c r="Q32" s="395"/>
+      <c r="I32" s="398"/>
+      <c r="J32" s="398"/>
+      <c r="K32" s="398"/>
+      <c r="L32" s="398"/>
+      <c r="M32" s="398"/>
+      <c r="N32" s="398"/>
+      <c r="O32" s="398"/>
+      <c r="P32" s="398"/>
+      <c r="Q32" s="398"/>
       <c r="R32" s="109">
         <f t="shared" si="2"/>
         <v>400.35</v>
@@ -13765,24 +13765,24 @@
       <c r="B33" s="121">
         <v>1958.28</v>
       </c>
-      <c r="C33" s="392"/>
-      <c r="D33" s="393"/>
-      <c r="E33" s="392"/>
-      <c r="F33" s="392"/>
-      <c r="G33" s="394"/>
+      <c r="C33" s="393"/>
+      <c r="D33" s="394"/>
+      <c r="E33" s="393"/>
+      <c r="F33" s="393"/>
+      <c r="G33" s="395"/>
       <c r="H33" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I33" s="395"/>
-      <c r="J33" s="395"/>
-      <c r="K33" s="395"/>
-      <c r="L33" s="395"/>
-      <c r="M33" s="395"/>
-      <c r="N33" s="395"/>
-      <c r="O33" s="395"/>
-      <c r="P33" s="395"/>
-      <c r="Q33" s="395"/>
+      <c r="I33" s="398"/>
+      <c r="J33" s="398"/>
+      <c r="K33" s="398"/>
+      <c r="L33" s="398"/>
+      <c r="M33" s="398"/>
+      <c r="N33" s="398"/>
+      <c r="O33" s="398"/>
+      <c r="P33" s="398"/>
+      <c r="Q33" s="398"/>
       <c r="R33" s="109">
         <f>R30</f>
         <v>400.35</v>
@@ -13795,24 +13795,24 @@
       <c r="B34" s="121">
         <v>2081.2600000000002</v>
       </c>
-      <c r="C34" s="392"/>
-      <c r="D34" s="393"/>
-      <c r="E34" s="392"/>
-      <c r="F34" s="392"/>
-      <c r="G34" s="394"/>
+      <c r="C34" s="393"/>
+      <c r="D34" s="394"/>
+      <c r="E34" s="393"/>
+      <c r="F34" s="393"/>
+      <c r="G34" s="395"/>
       <c r="H34" s="120">
         <f t="shared" si="1"/>
         <v>89.637500000000003</v>
       </c>
-      <c r="I34" s="395"/>
-      <c r="J34" s="395"/>
-      <c r="K34" s="395"/>
-      <c r="L34" s="395"/>
-      <c r="M34" s="395"/>
-      <c r="N34" s="395"/>
-      <c r="O34" s="395"/>
-      <c r="P34" s="395"/>
-      <c r="Q34" s="395"/>
+      <c r="I34" s="398"/>
+      <c r="J34" s="398"/>
+      <c r="K34" s="398"/>
+      <c r="L34" s="398"/>
+      <c r="M34" s="398"/>
+      <c r="N34" s="398"/>
+      <c r="O34" s="398"/>
+      <c r="P34" s="398"/>
+      <c r="Q34" s="398"/>
       <c r="R34" s="109">
         <f>R32</f>
         <v>400.35</v>
@@ -13828,38 +13828,38 @@
       <c r="B35" s="121">
         <v>2171.2600000000002</v>
       </c>
-      <c r="C35" s="392">
+      <c r="C35" s="393">
         <v>30.19</v>
       </c>
-      <c r="D35" s="393">
+      <c r="D35" s="394">
         <f>IF(B40&gt;0,SUM(B35:B40)-C35,0)</f>
         <v>13016.160000000002</v>
       </c>
-      <c r="E35" s="392">
+      <c r="E35" s="393">
         <v>6.1369999999999996</v>
       </c>
-      <c r="F35" s="392">
+      <c r="F35" s="393">
         <v>25.93</v>
       </c>
-      <c r="G35" s="394">
+      <c r="G35" s="395">
         <v>96</v>
       </c>
       <c r="H35" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I35" s="395">
+      <c r="I35" s="398">
         <f>IF($D$2&gt;F35,G35*($D$2-F35)*0.2,0)</f>
         <v>73.344000000000008</v>
       </c>
-      <c r="J35" s="395"/>
-      <c r="K35" s="395"/>
-      <c r="L35" s="395"/>
-      <c r="M35" s="395"/>
-      <c r="N35" s="395"/>
-      <c r="O35" s="395"/>
-      <c r="P35" s="395"/>
-      <c r="Q35" s="395"/>
+      <c r="J35" s="398"/>
+      <c r="K35" s="398"/>
+      <c r="L35" s="398"/>
+      <c r="M35" s="398"/>
+      <c r="N35" s="398"/>
+      <c r="O35" s="398"/>
+      <c r="P35" s="398"/>
+      <c r="Q35" s="398"/>
       <c r="R35" s="109">
         <v>358.55</v>
       </c>
@@ -13871,24 +13871,24 @@
       <c r="B36" s="121">
         <v>2081.27</v>
       </c>
-      <c r="C36" s="392"/>
-      <c r="D36" s="393"/>
-      <c r="E36" s="392"/>
-      <c r="F36" s="392"/>
-      <c r="G36" s="394"/>
+      <c r="C36" s="393"/>
+      <c r="D36" s="394"/>
+      <c r="E36" s="393"/>
+      <c r="F36" s="393"/>
+      <c r="G36" s="395"/>
       <c r="H36" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I36" s="395"/>
-      <c r="J36" s="395"/>
-      <c r="K36" s="395"/>
-      <c r="L36" s="395"/>
-      <c r="M36" s="395"/>
-      <c r="N36" s="395"/>
-      <c r="O36" s="395"/>
-      <c r="P36" s="395"/>
-      <c r="Q36" s="395"/>
+      <c r="I36" s="398"/>
+      <c r="J36" s="398"/>
+      <c r="K36" s="398"/>
+      <c r="L36" s="398"/>
+      <c r="M36" s="398"/>
+      <c r="N36" s="398"/>
+      <c r="O36" s="398"/>
+      <c r="P36" s="398"/>
+      <c r="Q36" s="398"/>
       <c r="R36" s="109">
         <v>358.55</v>
       </c>
@@ -13900,24 +13900,24 @@
       <c r="B37" s="121">
         <v>2081.2600000000002</v>
       </c>
-      <c r="C37" s="392"/>
-      <c r="D37" s="393"/>
-      <c r="E37" s="392"/>
-      <c r="F37" s="392"/>
-      <c r="G37" s="394"/>
+      <c r="C37" s="393"/>
+      <c r="D37" s="394"/>
+      <c r="E37" s="393"/>
+      <c r="F37" s="393"/>
+      <c r="G37" s="395"/>
       <c r="H37" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I37" s="395"/>
-      <c r="J37" s="395"/>
-      <c r="K37" s="395"/>
-      <c r="L37" s="395"/>
-      <c r="M37" s="395"/>
-      <c r="N37" s="395"/>
-      <c r="O37" s="395"/>
-      <c r="P37" s="395"/>
-      <c r="Q37" s="395"/>
+      <c r="I37" s="398"/>
+      <c r="J37" s="398"/>
+      <c r="K37" s="398"/>
+      <c r="L37" s="398"/>
+      <c r="M37" s="398"/>
+      <c r="N37" s="398"/>
+      <c r="O37" s="398"/>
+      <c r="P37" s="398"/>
+      <c r="Q37" s="398"/>
       <c r="R37" s="109">
         <v>358.55</v>
       </c>
@@ -13929,24 +13929,24 @@
       <c r="B38" s="121">
         <v>2537.5100000000002</v>
       </c>
-      <c r="C38" s="392"/>
-      <c r="D38" s="393"/>
-      <c r="E38" s="392"/>
-      <c r="F38" s="392"/>
-      <c r="G38" s="394"/>
+      <c r="C38" s="393"/>
+      <c r="D38" s="394"/>
+      <c r="E38" s="393"/>
+      <c r="F38" s="393"/>
+      <c r="G38" s="395"/>
       <c r="H38" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I38" s="395"/>
-      <c r="J38" s="395"/>
-      <c r="K38" s="395"/>
-      <c r="L38" s="395"/>
-      <c r="M38" s="395"/>
-      <c r="N38" s="395"/>
-      <c r="O38" s="395"/>
-      <c r="P38" s="395"/>
-      <c r="Q38" s="395"/>
+      <c r="I38" s="398"/>
+      <c r="J38" s="398"/>
+      <c r="K38" s="398"/>
+      <c r="L38" s="398"/>
+      <c r="M38" s="398"/>
+      <c r="N38" s="398"/>
+      <c r="O38" s="398"/>
+      <c r="P38" s="398"/>
+      <c r="Q38" s="398"/>
       <c r="R38" s="109">
         <v>358.55</v>
       </c>
@@ -13958,24 +13958,24 @@
       <c r="B39" s="121">
         <v>2087.52</v>
       </c>
-      <c r="C39" s="392"/>
-      <c r="D39" s="393"/>
-      <c r="E39" s="392"/>
-      <c r="F39" s="392"/>
-      <c r="G39" s="394"/>
+      <c r="C39" s="393"/>
+      <c r="D39" s="394"/>
+      <c r="E39" s="393"/>
+      <c r="F39" s="393"/>
+      <c r="G39" s="395"/>
       <c r="H39" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I39" s="395"/>
-      <c r="J39" s="395"/>
-      <c r="K39" s="395"/>
-      <c r="L39" s="395"/>
-      <c r="M39" s="395"/>
-      <c r="N39" s="395"/>
-      <c r="O39" s="395"/>
-      <c r="P39" s="395"/>
-      <c r="Q39" s="395"/>
+      <c r="I39" s="398"/>
+      <c r="J39" s="398"/>
+      <c r="K39" s="398"/>
+      <c r="L39" s="398"/>
+      <c r="M39" s="398"/>
+      <c r="N39" s="398"/>
+      <c r="O39" s="398"/>
+      <c r="P39" s="398"/>
+      <c r="Q39" s="398"/>
       <c r="R39" s="109">
         <v>358.55</v>
       </c>
@@ -13987,24 +13987,24 @@
       <c r="B40" s="121">
         <v>2087.5300000000002</v>
       </c>
-      <c r="C40" s="392"/>
-      <c r="D40" s="393"/>
-      <c r="E40" s="392"/>
-      <c r="F40" s="392"/>
-      <c r="G40" s="394"/>
+      <c r="C40" s="393"/>
+      <c r="D40" s="394"/>
+      <c r="E40" s="393"/>
+      <c r="F40" s="393"/>
+      <c r="G40" s="395"/>
       <c r="H40" s="120">
         <f t="shared" si="1"/>
         <v>95.492500000000007</v>
       </c>
-      <c r="I40" s="395"/>
-      <c r="J40" s="395"/>
-      <c r="K40" s="395"/>
-      <c r="L40" s="395"/>
-      <c r="M40" s="395"/>
-      <c r="N40" s="395"/>
-      <c r="O40" s="395"/>
-      <c r="P40" s="395"/>
-      <c r="Q40" s="395"/>
+      <c r="I40" s="398"/>
+      <c r="J40" s="398"/>
+      <c r="K40" s="398"/>
+      <c r="L40" s="398"/>
+      <c r="M40" s="398"/>
+      <c r="N40" s="398"/>
+      <c r="O40" s="398"/>
+      <c r="P40" s="398"/>
+      <c r="Q40" s="398"/>
       <c r="R40" s="109">
         <v>358.55</v>
       </c>
@@ -14016,38 +14016,38 @@
       <c r="B41" s="121">
         <v>2362.48</v>
       </c>
-      <c r="C41" s="392">
+      <c r="C41" s="393">
         <v>52.72</v>
       </c>
-      <c r="D41" s="393">
+      <c r="D41" s="394">
         <f>IF(B46&gt;0,SUM(B41:B46)-C41,0)</f>
         <v>13224.73</v>
       </c>
-      <c r="E41" s="392">
+      <c r="E41" s="393">
         <v>6.2213000000000003</v>
       </c>
-      <c r="F41" s="392">
+      <c r="F41" s="393">
         <v>26.89</v>
       </c>
-      <c r="G41" s="394">
+      <c r="G41" s="395">
         <v>93</v>
       </c>
       <c r="H41" s="120">
         <f t="shared" si="1"/>
         <v>95.527500000000003</v>
       </c>
-      <c r="I41" s="395">
+      <c r="I41" s="398">
         <f>IF($D$2&gt;F41,G41*($D$2-F41)*0.2,0)</f>
         <v>53.195999999999998</v>
       </c>
-      <c r="J41" s="395"/>
-      <c r="K41" s="395"/>
-      <c r="L41" s="395"/>
-      <c r="M41" s="395"/>
-      <c r="N41" s="395"/>
-      <c r="O41" s="395"/>
-      <c r="P41" s="395"/>
-      <c r="Q41" s="395"/>
+      <c r="J41" s="398"/>
+      <c r="K41" s="398"/>
+      <c r="L41" s="398"/>
+      <c r="M41" s="398"/>
+      <c r="N41" s="398"/>
+      <c r="O41" s="398"/>
+      <c r="P41" s="398"/>
+      <c r="Q41" s="398"/>
       <c r="R41" s="109">
         <v>381.97</v>
       </c>
@@ -14059,24 +14059,24 @@
       <c r="B42" s="121">
         <v>2174.98</v>
       </c>
-      <c r="C42" s="392"/>
-      <c r="D42" s="393"/>
-      <c r="E42" s="392"/>
-      <c r="F42" s="392"/>
-      <c r="G42" s="394"/>
+      <c r="C42" s="393"/>
+      <c r="D42" s="394"/>
+      <c r="E42" s="393"/>
+      <c r="F42" s="393"/>
+      <c r="G42" s="395"/>
       <c r="H42" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I42" s="395"/>
-      <c r="J42" s="395"/>
-      <c r="K42" s="395"/>
-      <c r="L42" s="395"/>
-      <c r="M42" s="395"/>
-      <c r="N42" s="395"/>
-      <c r="O42" s="395"/>
-      <c r="P42" s="395"/>
-      <c r="Q42" s="395"/>
+      <c r="I42" s="398"/>
+      <c r="J42" s="398"/>
+      <c r="K42" s="398"/>
+      <c r="L42" s="398"/>
+      <c r="M42" s="398"/>
+      <c r="N42" s="398"/>
+      <c r="O42" s="398"/>
+      <c r="P42" s="398"/>
+      <c r="Q42" s="398"/>
       <c r="R42" s="109">
         <v>381.97</v>
       </c>
@@ -14088,24 +14088,24 @@
       <c r="B43" s="121">
         <v>2265</v>
       </c>
-      <c r="C43" s="392"/>
-      <c r="D43" s="393"/>
-      <c r="E43" s="392"/>
-      <c r="F43" s="392"/>
-      <c r="G43" s="394"/>
+      <c r="C43" s="393"/>
+      <c r="D43" s="394"/>
+      <c r="E43" s="393"/>
+      <c r="F43" s="393"/>
+      <c r="G43" s="395"/>
       <c r="H43" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I43" s="395"/>
-      <c r="J43" s="395"/>
-      <c r="K43" s="395"/>
-      <c r="L43" s="395"/>
-      <c r="M43" s="395"/>
-      <c r="N43" s="395"/>
-      <c r="O43" s="395"/>
-      <c r="P43" s="395"/>
-      <c r="Q43" s="395"/>
+      <c r="I43" s="398"/>
+      <c r="J43" s="398"/>
+      <c r="K43" s="398"/>
+      <c r="L43" s="398"/>
+      <c r="M43" s="398"/>
+      <c r="N43" s="398"/>
+      <c r="O43" s="398"/>
+      <c r="P43" s="398"/>
+      <c r="Q43" s="398"/>
       <c r="R43" s="109">
         <v>381.97</v>
       </c>
@@ -14117,24 +14117,24 @@
       <c r="B44" s="121">
         <v>2087.5</v>
       </c>
-      <c r="C44" s="392"/>
-      <c r="D44" s="393"/>
-      <c r="E44" s="392"/>
-      <c r="F44" s="392"/>
-      <c r="G44" s="394"/>
+      <c r="C44" s="393"/>
+      <c r="D44" s="394"/>
+      <c r="E44" s="393"/>
+      <c r="F44" s="393"/>
+      <c r="G44" s="395"/>
       <c r="H44" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I44" s="395"/>
-      <c r="J44" s="395"/>
-      <c r="K44" s="395"/>
-      <c r="L44" s="395"/>
-      <c r="M44" s="395"/>
-      <c r="N44" s="395"/>
-      <c r="O44" s="395"/>
-      <c r="P44" s="395"/>
-      <c r="Q44" s="395"/>
+      <c r="I44" s="398"/>
+      <c r="J44" s="398"/>
+      <c r="K44" s="398"/>
+      <c r="L44" s="398"/>
+      <c r="M44" s="398"/>
+      <c r="N44" s="398"/>
+      <c r="O44" s="398"/>
+      <c r="P44" s="398"/>
+      <c r="Q44" s="398"/>
       <c r="R44" s="109">
         <v>381.97</v>
       </c>
@@ -14146,24 +14146,24 @@
       <c r="B45" s="121">
         <v>2087.48</v>
       </c>
-      <c r="C45" s="392"/>
-      <c r="D45" s="393"/>
-      <c r="E45" s="392"/>
-      <c r="F45" s="392"/>
-      <c r="G45" s="394"/>
+      <c r="C45" s="393"/>
+      <c r="D45" s="394"/>
+      <c r="E45" s="393"/>
+      <c r="F45" s="393"/>
+      <c r="G45" s="395"/>
       <c r="H45" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I45" s="395"/>
-      <c r="J45" s="395"/>
-      <c r="K45" s="395"/>
-      <c r="L45" s="395"/>
-      <c r="M45" s="395"/>
-      <c r="N45" s="395"/>
-      <c r="O45" s="395"/>
-      <c r="P45" s="395"/>
-      <c r="Q45" s="395"/>
+      <c r="I45" s="398"/>
+      <c r="J45" s="398"/>
+      <c r="K45" s="398"/>
+      <c r="L45" s="398"/>
+      <c r="M45" s="398"/>
+      <c r="N45" s="398"/>
+      <c r="O45" s="398"/>
+      <c r="P45" s="398"/>
+      <c r="Q45" s="398"/>
       <c r="R45" s="109">
         <v>381.97</v>
       </c>
@@ -14175,24 +14175,24 @@
       <c r="B46" s="121">
         <v>2300.0100000000002</v>
       </c>
-      <c r="C46" s="392"/>
-      <c r="D46" s="393"/>
-      <c r="E46" s="392"/>
-      <c r="F46" s="392"/>
-      <c r="G46" s="394"/>
+      <c r="C46" s="393"/>
+      <c r="D46" s="394"/>
+      <c r="E46" s="393"/>
+      <c r="F46" s="393"/>
+      <c r="G46" s="395"/>
       <c r="H46" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I46" s="395"/>
-      <c r="J46" s="395"/>
-      <c r="K46" s="395"/>
-      <c r="L46" s="395"/>
-      <c r="M46" s="395"/>
-      <c r="N46" s="395"/>
-      <c r="O46" s="395"/>
-      <c r="P46" s="395"/>
-      <c r="Q46" s="395"/>
+      <c r="I46" s="398"/>
+      <c r="J46" s="398"/>
+      <c r="K46" s="398"/>
+      <c r="L46" s="398"/>
+      <c r="M46" s="398"/>
+      <c r="N46" s="398"/>
+      <c r="O46" s="398"/>
+      <c r="P46" s="398"/>
+      <c r="Q46" s="398"/>
       <c r="R46" s="109">
         <v>381.97</v>
       </c>
@@ -14204,38 +14204,38 @@
       <c r="B47" s="121">
         <v>3787.17</v>
       </c>
-      <c r="C47" s="392">
-        <v>0</v>
-      </c>
-      <c r="D47" s="393">
+      <c r="C47" s="393">
+        <v>0</v>
+      </c>
+      <c r="D47" s="394">
         <f>IF(B52&gt;0,SUM(B47:B52)-C47,0)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="392">
+      <c r="E47" s="393">
         <v>6.2</v>
       </c>
-      <c r="F47" s="392">
+      <c r="F47" s="393">
         <v>25.3</v>
       </c>
-      <c r="G47" s="394">
+      <c r="G47" s="395">
         <v>0</v>
       </c>
       <c r="H47" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I47" s="395">
+      <c r="I47" s="398">
         <f>IF($D$2&gt;F47,G47*($D$2-F47)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J47" s="395"/>
-      <c r="K47" s="395"/>
-      <c r="L47" s="395"/>
-      <c r="M47" s="395"/>
-      <c r="N47" s="395"/>
-      <c r="O47" s="395"/>
-      <c r="P47" s="395"/>
-      <c r="Q47" s="395"/>
+      <c r="J47" s="398"/>
+      <c r="K47" s="398"/>
+      <c r="L47" s="398"/>
+      <c r="M47" s="398"/>
+      <c r="N47" s="398"/>
+      <c r="O47" s="398"/>
+      <c r="P47" s="398"/>
+      <c r="Q47" s="398"/>
       <c r="R47" s="109">
         <v>382.11</v>
       </c>
@@ -14247,24 +14247,24 @@
       <c r="B48" s="121">
         <v>0</v>
       </c>
-      <c r="C48" s="392"/>
-      <c r="D48" s="393"/>
-      <c r="E48" s="392"/>
-      <c r="F48" s="392"/>
-      <c r="G48" s="394"/>
+      <c r="C48" s="393"/>
+      <c r="D48" s="394"/>
+      <c r="E48" s="393"/>
+      <c r="F48" s="393"/>
+      <c r="G48" s="395"/>
       <c r="H48" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I48" s="395"/>
-      <c r="J48" s="395"/>
-      <c r="K48" s="395"/>
-      <c r="L48" s="395"/>
-      <c r="M48" s="395"/>
-      <c r="N48" s="395"/>
-      <c r="O48" s="395"/>
-      <c r="P48" s="395"/>
-      <c r="Q48" s="395"/>
+      <c r="I48" s="398"/>
+      <c r="J48" s="398"/>
+      <c r="K48" s="398"/>
+      <c r="L48" s="398"/>
+      <c r="M48" s="398"/>
+      <c r="N48" s="398"/>
+      <c r="O48" s="398"/>
+      <c r="P48" s="398"/>
+      <c r="Q48" s="398"/>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="1">
@@ -14273,24 +14273,24 @@
       <c r="B49" s="121">
         <v>0</v>
       </c>
-      <c r="C49" s="392"/>
-      <c r="D49" s="393"/>
-      <c r="E49" s="392"/>
-      <c r="F49" s="392"/>
-      <c r="G49" s="394"/>
+      <c r="C49" s="393"/>
+      <c r="D49" s="394"/>
+      <c r="E49" s="393"/>
+      <c r="F49" s="393"/>
+      <c r="G49" s="395"/>
       <c r="H49" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I49" s="395"/>
-      <c r="J49" s="395"/>
-      <c r="K49" s="395"/>
-      <c r="L49" s="395"/>
-      <c r="M49" s="395"/>
-      <c r="N49" s="395"/>
-      <c r="O49" s="395"/>
-      <c r="P49" s="395"/>
-      <c r="Q49" s="395"/>
+      <c r="I49" s="398"/>
+      <c r="J49" s="398"/>
+      <c r="K49" s="398"/>
+      <c r="L49" s="398"/>
+      <c r="M49" s="398"/>
+      <c r="N49" s="398"/>
+      <c r="O49" s="398"/>
+      <c r="P49" s="398"/>
+      <c r="Q49" s="398"/>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" s="1">
@@ -14299,24 +14299,24 @@
       <c r="B50" s="121">
         <v>0</v>
       </c>
-      <c r="C50" s="392"/>
-      <c r="D50" s="393"/>
-      <c r="E50" s="392"/>
-      <c r="F50" s="392"/>
-      <c r="G50" s="394"/>
+      <c r="C50" s="393"/>
+      <c r="D50" s="394"/>
+      <c r="E50" s="393"/>
+      <c r="F50" s="393"/>
+      <c r="G50" s="395"/>
       <c r="H50" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I50" s="395"/>
-      <c r="J50" s="395"/>
-      <c r="K50" s="395"/>
-      <c r="L50" s="395"/>
-      <c r="M50" s="395"/>
-      <c r="N50" s="395"/>
-      <c r="O50" s="395"/>
-      <c r="P50" s="395"/>
-      <c r="Q50" s="395"/>
+      <c r="I50" s="398"/>
+      <c r="J50" s="398"/>
+      <c r="K50" s="398"/>
+      <c r="L50" s="398"/>
+      <c r="M50" s="398"/>
+      <c r="N50" s="398"/>
+      <c r="O50" s="398"/>
+      <c r="P50" s="398"/>
+      <c r="Q50" s="398"/>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="1">
@@ -14325,24 +14325,24 @@
       <c r="B51" s="121">
         <v>0</v>
       </c>
-      <c r="C51" s="392"/>
-      <c r="D51" s="393"/>
-      <c r="E51" s="392"/>
-      <c r="F51" s="392"/>
-      <c r="G51" s="394"/>
+      <c r="C51" s="393"/>
+      <c r="D51" s="394"/>
+      <c r="E51" s="393"/>
+      <c r="F51" s="393"/>
+      <c r="G51" s="395"/>
       <c r="H51" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I51" s="395"/>
-      <c r="J51" s="395"/>
-      <c r="K51" s="395"/>
-      <c r="L51" s="395"/>
-      <c r="M51" s="395"/>
-      <c r="N51" s="395"/>
-      <c r="O51" s="395"/>
-      <c r="P51" s="395"/>
-      <c r="Q51" s="395"/>
+      <c r="I51" s="398"/>
+      <c r="J51" s="398"/>
+      <c r="K51" s="398"/>
+      <c r="L51" s="398"/>
+      <c r="M51" s="398"/>
+      <c r="N51" s="398"/>
+      <c r="O51" s="398"/>
+      <c r="P51" s="398"/>
+      <c r="Q51" s="398"/>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="1">
@@ -14351,24 +14351,24 @@
       <c r="B52" s="121">
         <v>0</v>
       </c>
-      <c r="C52" s="392"/>
-      <c r="D52" s="393"/>
-      <c r="E52" s="392"/>
-      <c r="F52" s="392"/>
-      <c r="G52" s="394"/>
+      <c r="C52" s="393"/>
+      <c r="D52" s="394"/>
+      <c r="E52" s="393"/>
+      <c r="F52" s="393"/>
+      <c r="G52" s="395"/>
       <c r="H52" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I52" s="395"/>
-      <c r="J52" s="395"/>
-      <c r="K52" s="395"/>
-      <c r="L52" s="395"/>
-      <c r="M52" s="395"/>
-      <c r="N52" s="395"/>
-      <c r="O52" s="395"/>
-      <c r="P52" s="395"/>
-      <c r="Q52" s="395"/>
+      <c r="I52" s="398"/>
+      <c r="J52" s="398"/>
+      <c r="K52" s="398"/>
+      <c r="L52" s="398"/>
+      <c r="M52" s="398"/>
+      <c r="N52" s="398"/>
+      <c r="O52" s="398"/>
+      <c r="P52" s="398"/>
+      <c r="Q52" s="398"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="1">
@@ -14377,38 +14377,38 @@
       <c r="B53" s="121">
         <v>0</v>
       </c>
-      <c r="C53" s="392">
-        <v>0</v>
-      </c>
-      <c r="D53" s="393">
+      <c r="C53" s="393">
+        <v>0</v>
+      </c>
+      <c r="D53" s="394">
         <f>IF(B58&gt;0,SUM(B53:B58)-C53,0)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="392">
+      <c r="E53" s="393">
         <v>6.2</v>
       </c>
-      <c r="F53" s="392">
+      <c r="F53" s="393">
         <v>25.3</v>
       </c>
-      <c r="G53" s="394">
+      <c r="G53" s="395">
         <v>0</v>
       </c>
       <c r="H53" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I53" s="395">
+      <c r="I53" s="398">
         <f>IF($D$2&gt;F53,G53*($D$2-F53)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J53" s="395"/>
-      <c r="K53" s="395"/>
-      <c r="L53" s="395"/>
-      <c r="M53" s="395"/>
-      <c r="N53" s="395"/>
-      <c r="O53" s="395"/>
-      <c r="P53" s="395"/>
-      <c r="Q53" s="395"/>
+      <c r="J53" s="398"/>
+      <c r="K53" s="398"/>
+      <c r="L53" s="398"/>
+      <c r="M53" s="398"/>
+      <c r="N53" s="398"/>
+      <c r="O53" s="398"/>
+      <c r="P53" s="398"/>
+      <c r="Q53" s="398"/>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="1">
@@ -14417,24 +14417,24 @@
       <c r="B54" s="121">
         <v>0</v>
       </c>
-      <c r="C54" s="392"/>
-      <c r="D54" s="393"/>
-      <c r="E54" s="392"/>
-      <c r="F54" s="392"/>
-      <c r="G54" s="394"/>
+      <c r="C54" s="393"/>
+      <c r="D54" s="394"/>
+      <c r="E54" s="393"/>
+      <c r="F54" s="393"/>
+      <c r="G54" s="395"/>
       <c r="H54" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I54" s="395"/>
-      <c r="J54" s="395"/>
-      <c r="K54" s="395"/>
-      <c r="L54" s="395"/>
-      <c r="M54" s="395"/>
-      <c r="N54" s="395"/>
-      <c r="O54" s="395"/>
-      <c r="P54" s="395"/>
-      <c r="Q54" s="395"/>
+      <c r="I54" s="398"/>
+      <c r="J54" s="398"/>
+      <c r="K54" s="398"/>
+      <c r="L54" s="398"/>
+      <c r="M54" s="398"/>
+      <c r="N54" s="398"/>
+      <c r="O54" s="398"/>
+      <c r="P54" s="398"/>
+      <c r="Q54" s="398"/>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="1">
@@ -14443,24 +14443,24 @@
       <c r="B55" s="121">
         <v>0</v>
       </c>
-      <c r="C55" s="392"/>
-      <c r="D55" s="393"/>
-      <c r="E55" s="392"/>
-      <c r="F55" s="392"/>
-      <c r="G55" s="394"/>
+      <c r="C55" s="393"/>
+      <c r="D55" s="394"/>
+      <c r="E55" s="393"/>
+      <c r="F55" s="393"/>
+      <c r="G55" s="395"/>
       <c r="H55" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I55" s="395"/>
-      <c r="J55" s="395"/>
-      <c r="K55" s="395"/>
-      <c r="L55" s="395"/>
-      <c r="M55" s="395"/>
-      <c r="N55" s="395"/>
-      <c r="O55" s="395"/>
-      <c r="P55" s="395"/>
-      <c r="Q55" s="395"/>
+      <c r="I55" s="398"/>
+      <c r="J55" s="398"/>
+      <c r="K55" s="398"/>
+      <c r="L55" s="398"/>
+      <c r="M55" s="398"/>
+      <c r="N55" s="398"/>
+      <c r="O55" s="398"/>
+      <c r="P55" s="398"/>
+      <c r="Q55" s="398"/>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="1">
@@ -14469,24 +14469,24 @@
       <c r="B56" s="121">
         <v>0</v>
       </c>
-      <c r="C56" s="392"/>
-      <c r="D56" s="393"/>
-      <c r="E56" s="392"/>
-      <c r="F56" s="392"/>
-      <c r="G56" s="394"/>
+      <c r="C56" s="393"/>
+      <c r="D56" s="394"/>
+      <c r="E56" s="393"/>
+      <c r="F56" s="393"/>
+      <c r="G56" s="395"/>
       <c r="H56" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I56" s="395"/>
-      <c r="J56" s="395"/>
-      <c r="K56" s="395"/>
-      <c r="L56" s="395"/>
-      <c r="M56" s="395"/>
-      <c r="N56" s="395"/>
-      <c r="O56" s="395"/>
-      <c r="P56" s="395"/>
-      <c r="Q56" s="395"/>
+      <c r="I56" s="398"/>
+      <c r="J56" s="398"/>
+      <c r="K56" s="398"/>
+      <c r="L56" s="398"/>
+      <c r="M56" s="398"/>
+      <c r="N56" s="398"/>
+      <c r="O56" s="398"/>
+      <c r="P56" s="398"/>
+      <c r="Q56" s="398"/>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" s="1">
@@ -14495,24 +14495,24 @@
       <c r="B57" s="121">
         <v>0</v>
       </c>
-      <c r="C57" s="392"/>
-      <c r="D57" s="393"/>
-      <c r="E57" s="392"/>
-      <c r="F57" s="392"/>
-      <c r="G57" s="394"/>
+      <c r="C57" s="393"/>
+      <c r="D57" s="394"/>
+      <c r="E57" s="393"/>
+      <c r="F57" s="393"/>
+      <c r="G57" s="395"/>
       <c r="H57" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I57" s="395"/>
-      <c r="J57" s="395"/>
-      <c r="K57" s="395"/>
-      <c r="L57" s="395"/>
-      <c r="M57" s="395"/>
-      <c r="N57" s="395"/>
-      <c r="O57" s="395"/>
-      <c r="P57" s="395"/>
-      <c r="Q57" s="395"/>
+      <c r="I57" s="398"/>
+      <c r="J57" s="398"/>
+      <c r="K57" s="398"/>
+      <c r="L57" s="398"/>
+      <c r="M57" s="398"/>
+      <c r="N57" s="398"/>
+      <c r="O57" s="398"/>
+      <c r="P57" s="398"/>
+      <c r="Q57" s="398"/>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="1">
@@ -14521,24 +14521,24 @@
       <c r="B58" s="121">
         <v>0</v>
       </c>
-      <c r="C58" s="392"/>
-      <c r="D58" s="393"/>
-      <c r="E58" s="392"/>
-      <c r="F58" s="392"/>
-      <c r="G58" s="394"/>
+      <c r="C58" s="393"/>
+      <c r="D58" s="394"/>
+      <c r="E58" s="393"/>
+      <c r="F58" s="393"/>
+      <c r="G58" s="395"/>
       <c r="H58" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I58" s="395"/>
-      <c r="J58" s="395"/>
-      <c r="K58" s="395"/>
-      <c r="L58" s="395"/>
-      <c r="M58" s="395"/>
-      <c r="N58" s="395"/>
-      <c r="O58" s="395"/>
-      <c r="P58" s="395"/>
-      <c r="Q58" s="395"/>
+      <c r="I58" s="398"/>
+      <c r="J58" s="398"/>
+      <c r="K58" s="398"/>
+      <c r="L58" s="398"/>
+      <c r="M58" s="398"/>
+      <c r="N58" s="398"/>
+      <c r="O58" s="398"/>
+      <c r="P58" s="398"/>
+      <c r="Q58" s="398"/>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="1">
@@ -14547,38 +14547,38 @@
       <c r="B59" s="121">
         <v>0</v>
       </c>
-      <c r="C59" s="392">
-        <v>0</v>
-      </c>
-      <c r="D59" s="393">
+      <c r="C59" s="393">
+        <v>0</v>
+      </c>
+      <c r="D59" s="394">
         <f>IF(B64&gt;0,SUM(B59:B64)-C59,0)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="392">
+      <c r="E59" s="393">
         <v>6.2</v>
       </c>
-      <c r="F59" s="392">
+      <c r="F59" s="393">
         <v>25.3</v>
       </c>
-      <c r="G59" s="394">
+      <c r="G59" s="395">
         <v>0</v>
       </c>
       <c r="H59" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I59" s="395">
+      <c r="I59" s="398">
         <f>IF($D$2&gt;F59,G59*($D$2-F59)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J59" s="395"/>
-      <c r="K59" s="395"/>
-      <c r="L59" s="395"/>
-      <c r="M59" s="395"/>
-      <c r="N59" s="395"/>
-      <c r="O59" s="395"/>
-      <c r="P59" s="395"/>
-      <c r="Q59" s="395"/>
+      <c r="J59" s="398"/>
+      <c r="K59" s="398"/>
+      <c r="L59" s="398"/>
+      <c r="M59" s="398"/>
+      <c r="N59" s="398"/>
+      <c r="O59" s="398"/>
+      <c r="P59" s="398"/>
+      <c r="Q59" s="398"/>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="1">
@@ -14587,24 +14587,24 @@
       <c r="B60" s="121">
         <v>0</v>
       </c>
-      <c r="C60" s="392"/>
-      <c r="D60" s="393"/>
-      <c r="E60" s="392"/>
-      <c r="F60" s="392"/>
-      <c r="G60" s="394"/>
+      <c r="C60" s="393"/>
+      <c r="D60" s="394"/>
+      <c r="E60" s="393"/>
+      <c r="F60" s="393"/>
+      <c r="G60" s="395"/>
       <c r="H60" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I60" s="395"/>
-      <c r="J60" s="395"/>
-      <c r="K60" s="395"/>
-      <c r="L60" s="395"/>
-      <c r="M60" s="395"/>
-      <c r="N60" s="395"/>
-      <c r="O60" s="395"/>
-      <c r="P60" s="395"/>
-      <c r="Q60" s="395"/>
+      <c r="I60" s="398"/>
+      <c r="J60" s="398"/>
+      <c r="K60" s="398"/>
+      <c r="L60" s="398"/>
+      <c r="M60" s="398"/>
+      <c r="N60" s="398"/>
+      <c r="O60" s="398"/>
+      <c r="P60" s="398"/>
+      <c r="Q60" s="398"/>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="1">
@@ -14613,24 +14613,24 @@
       <c r="B61" s="121">
         <v>0</v>
       </c>
-      <c r="C61" s="392"/>
-      <c r="D61" s="393"/>
-      <c r="E61" s="392"/>
-      <c r="F61" s="392"/>
-      <c r="G61" s="394"/>
+      <c r="C61" s="393"/>
+      <c r="D61" s="394"/>
+      <c r="E61" s="393"/>
+      <c r="F61" s="393"/>
+      <c r="G61" s="395"/>
       <c r="H61" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I61" s="395"/>
-      <c r="J61" s="395"/>
-      <c r="K61" s="395"/>
-      <c r="L61" s="395"/>
-      <c r="M61" s="395"/>
-      <c r="N61" s="395"/>
-      <c r="O61" s="395"/>
-      <c r="P61" s="395"/>
-      <c r="Q61" s="395"/>
+      <c r="I61" s="398"/>
+      <c r="J61" s="398"/>
+      <c r="K61" s="398"/>
+      <c r="L61" s="398"/>
+      <c r="M61" s="398"/>
+      <c r="N61" s="398"/>
+      <c r="O61" s="398"/>
+      <c r="P61" s="398"/>
+      <c r="Q61" s="398"/>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" s="1">
@@ -14639,24 +14639,24 @@
       <c r="B62" s="121">
         <v>0</v>
       </c>
-      <c r="C62" s="392"/>
-      <c r="D62" s="393"/>
-      <c r="E62" s="392"/>
-      <c r="F62" s="392"/>
-      <c r="G62" s="394"/>
+      <c r="C62" s="393"/>
+      <c r="D62" s="394"/>
+      <c r="E62" s="393"/>
+      <c r="F62" s="393"/>
+      <c r="G62" s="395"/>
       <c r="H62" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I62" s="395"/>
-      <c r="J62" s="395"/>
-      <c r="K62" s="395"/>
-      <c r="L62" s="395"/>
-      <c r="M62" s="395"/>
-      <c r="N62" s="395"/>
-      <c r="O62" s="395"/>
-      <c r="P62" s="395"/>
-      <c r="Q62" s="395"/>
+      <c r="I62" s="398"/>
+      <c r="J62" s="398"/>
+      <c r="K62" s="398"/>
+      <c r="L62" s="398"/>
+      <c r="M62" s="398"/>
+      <c r="N62" s="398"/>
+      <c r="O62" s="398"/>
+      <c r="P62" s="398"/>
+      <c r="Q62" s="398"/>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="1">
@@ -14665,24 +14665,24 @@
       <c r="B63" s="121">
         <v>0</v>
       </c>
-      <c r="C63" s="392"/>
-      <c r="D63" s="393"/>
-      <c r="E63" s="392"/>
-      <c r="F63" s="392"/>
-      <c r="G63" s="394"/>
+      <c r="C63" s="393"/>
+      <c r="D63" s="394"/>
+      <c r="E63" s="393"/>
+      <c r="F63" s="393"/>
+      <c r="G63" s="395"/>
       <c r="H63" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I63" s="395"/>
-      <c r="J63" s="395"/>
-      <c r="K63" s="395"/>
-      <c r="L63" s="395"/>
-      <c r="M63" s="395"/>
-      <c r="N63" s="395"/>
-      <c r="O63" s="395"/>
-      <c r="P63" s="395"/>
-      <c r="Q63" s="395"/>
+      <c r="I63" s="398"/>
+      <c r="J63" s="398"/>
+      <c r="K63" s="398"/>
+      <c r="L63" s="398"/>
+      <c r="M63" s="398"/>
+      <c r="N63" s="398"/>
+      <c r="O63" s="398"/>
+      <c r="P63" s="398"/>
+      <c r="Q63" s="398"/>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="1">
@@ -14691,24 +14691,24 @@
       <c r="B64" s="121">
         <v>0</v>
       </c>
-      <c r="C64" s="392"/>
-      <c r="D64" s="393"/>
-      <c r="E64" s="392"/>
-      <c r="F64" s="392"/>
-      <c r="G64" s="394"/>
+      <c r="C64" s="393"/>
+      <c r="D64" s="394"/>
+      <c r="E64" s="393"/>
+      <c r="F64" s="393"/>
+      <c r="G64" s="395"/>
       <c r="H64" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I64" s="395"/>
-      <c r="J64" s="395"/>
-      <c r="K64" s="395"/>
-      <c r="L64" s="395"/>
-      <c r="M64" s="395"/>
-      <c r="N64" s="395"/>
-      <c r="O64" s="395"/>
-      <c r="P64" s="395"/>
-      <c r="Q64" s="395"/>
+      <c r="I64" s="398"/>
+      <c r="J64" s="398"/>
+      <c r="K64" s="398"/>
+      <c r="L64" s="398"/>
+      <c r="M64" s="398"/>
+      <c r="N64" s="398"/>
+      <c r="O64" s="398"/>
+      <c r="P64" s="398"/>
+      <c r="Q64" s="398"/>
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="1">
@@ -14717,38 +14717,38 @@
       <c r="B65" s="121">
         <v>0</v>
       </c>
-      <c r="C65" s="392">
-        <v>0</v>
-      </c>
-      <c r="D65" s="393">
+      <c r="C65" s="393">
+        <v>0</v>
+      </c>
+      <c r="D65" s="394">
         <f>IF(B70&gt;0,SUM(B65:B70)-C65,0)</f>
         <v>0</v>
       </c>
-      <c r="E65" s="392">
+      <c r="E65" s="393">
         <v>6.2</v>
       </c>
-      <c r="F65" s="392">
+      <c r="F65" s="393">
         <v>25.3</v>
       </c>
-      <c r="G65" s="394">
+      <c r="G65" s="395">
         <v>0</v>
       </c>
       <c r="H65" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I65" s="395">
+      <c r="I65" s="398">
         <f>IF($D$2&gt;F65,G65*($D$2-F65)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J65" s="395"/>
-      <c r="K65" s="395"/>
-      <c r="L65" s="395"/>
-      <c r="M65" s="395"/>
-      <c r="N65" s="395"/>
-      <c r="O65" s="395"/>
-      <c r="P65" s="395"/>
-      <c r="Q65" s="395"/>
+      <c r="J65" s="398"/>
+      <c r="K65" s="398"/>
+      <c r="L65" s="398"/>
+      <c r="M65" s="398"/>
+      <c r="N65" s="398"/>
+      <c r="O65" s="398"/>
+      <c r="P65" s="398"/>
+      <c r="Q65" s="398"/>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="1">
@@ -14757,24 +14757,24 @@
       <c r="B66" s="121">
         <v>0</v>
       </c>
-      <c r="C66" s="392"/>
-      <c r="D66" s="393"/>
-      <c r="E66" s="392"/>
-      <c r="F66" s="392"/>
-      <c r="G66" s="394"/>
+      <c r="C66" s="393"/>
+      <c r="D66" s="394"/>
+      <c r="E66" s="393"/>
+      <c r="F66" s="393"/>
+      <c r="G66" s="395"/>
       <c r="H66" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I66" s="395"/>
-      <c r="J66" s="395"/>
-      <c r="K66" s="395"/>
-      <c r="L66" s="395"/>
-      <c r="M66" s="395"/>
-      <c r="N66" s="395"/>
-      <c r="O66" s="395"/>
-      <c r="P66" s="395"/>
-      <c r="Q66" s="395"/>
+      <c r="I66" s="398"/>
+      <c r="J66" s="398"/>
+      <c r="K66" s="398"/>
+      <c r="L66" s="398"/>
+      <c r="M66" s="398"/>
+      <c r="N66" s="398"/>
+      <c r="O66" s="398"/>
+      <c r="P66" s="398"/>
+      <c r="Q66" s="398"/>
     </row>
     <row r="67" spans="1:17">
       <c r="A67" s="1">
@@ -14783,24 +14783,24 @@
       <c r="B67" s="121">
         <v>0</v>
       </c>
-      <c r="C67" s="392"/>
-      <c r="D67" s="393"/>
-      <c r="E67" s="392"/>
-      <c r="F67" s="392"/>
-      <c r="G67" s="394"/>
+      <c r="C67" s="393"/>
+      <c r="D67" s="394"/>
+      <c r="E67" s="393"/>
+      <c r="F67" s="393"/>
+      <c r="G67" s="395"/>
       <c r="H67" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I67" s="395"/>
-      <c r="J67" s="395"/>
-      <c r="K67" s="395"/>
-      <c r="L67" s="395"/>
-      <c r="M67" s="395"/>
-      <c r="N67" s="395"/>
-      <c r="O67" s="395"/>
-      <c r="P67" s="395"/>
-      <c r="Q67" s="395"/>
+      <c r="I67" s="398"/>
+      <c r="J67" s="398"/>
+      <c r="K67" s="398"/>
+      <c r="L67" s="398"/>
+      <c r="M67" s="398"/>
+      <c r="N67" s="398"/>
+      <c r="O67" s="398"/>
+      <c r="P67" s="398"/>
+      <c r="Q67" s="398"/>
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="1">
@@ -14809,24 +14809,24 @@
       <c r="B68" s="121">
         <v>0</v>
       </c>
-      <c r="C68" s="392"/>
-      <c r="D68" s="393"/>
-      <c r="E68" s="392"/>
-      <c r="F68" s="392"/>
-      <c r="G68" s="394"/>
+      <c r="C68" s="393"/>
+      <c r="D68" s="394"/>
+      <c r="E68" s="393"/>
+      <c r="F68" s="393"/>
+      <c r="G68" s="395"/>
       <c r="H68" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I68" s="395"/>
-      <c r="J68" s="395"/>
-      <c r="K68" s="395"/>
-      <c r="L68" s="395"/>
-      <c r="M68" s="395"/>
-      <c r="N68" s="395"/>
-      <c r="O68" s="395"/>
-      <c r="P68" s="395"/>
-      <c r="Q68" s="395"/>
+      <c r="I68" s="398"/>
+      <c r="J68" s="398"/>
+      <c r="K68" s="398"/>
+      <c r="L68" s="398"/>
+      <c r="M68" s="398"/>
+      <c r="N68" s="398"/>
+      <c r="O68" s="398"/>
+      <c r="P68" s="398"/>
+      <c r="Q68" s="398"/>
     </row>
     <row r="69" spans="1:17">
       <c r="A69" s="1">
@@ -14835,24 +14835,24 @@
       <c r="B69" s="121">
         <v>0</v>
       </c>
-      <c r="C69" s="392"/>
-      <c r="D69" s="393"/>
-      <c r="E69" s="392"/>
-      <c r="F69" s="392"/>
-      <c r="G69" s="394"/>
+      <c r="C69" s="393"/>
+      <c r="D69" s="394"/>
+      <c r="E69" s="393"/>
+      <c r="F69" s="393"/>
+      <c r="G69" s="395"/>
       <c r="H69" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I69" s="395"/>
-      <c r="J69" s="395"/>
-      <c r="K69" s="395"/>
-      <c r="L69" s="395"/>
-      <c r="M69" s="395"/>
-      <c r="N69" s="395"/>
-      <c r="O69" s="395"/>
-      <c r="P69" s="395"/>
-      <c r="Q69" s="395"/>
+      <c r="I69" s="398"/>
+      <c r="J69" s="398"/>
+      <c r="K69" s="398"/>
+      <c r="L69" s="398"/>
+      <c r="M69" s="398"/>
+      <c r="N69" s="398"/>
+      <c r="O69" s="398"/>
+      <c r="P69" s="398"/>
+      <c r="Q69" s="398"/>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="1">
@@ -14861,24 +14861,24 @@
       <c r="B70" s="121">
         <v>0</v>
       </c>
-      <c r="C70" s="392"/>
-      <c r="D70" s="393"/>
-      <c r="E70" s="392"/>
-      <c r="F70" s="392"/>
-      <c r="G70" s="394"/>
+      <c r="C70" s="393"/>
+      <c r="D70" s="394"/>
+      <c r="E70" s="393"/>
+      <c r="F70" s="393"/>
+      <c r="G70" s="395"/>
       <c r="H70" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I70" s="395"/>
-      <c r="J70" s="395"/>
-      <c r="K70" s="395"/>
-      <c r="L70" s="395"/>
-      <c r="M70" s="395"/>
-      <c r="N70" s="395"/>
-      <c r="O70" s="395"/>
-      <c r="P70" s="395"/>
-      <c r="Q70" s="395"/>
+      <c r="I70" s="398"/>
+      <c r="J70" s="398"/>
+      <c r="K70" s="398"/>
+      <c r="L70" s="398"/>
+      <c r="M70" s="398"/>
+      <c r="N70" s="398"/>
+      <c r="O70" s="398"/>
+      <c r="P70" s="398"/>
+      <c r="Q70" s="398"/>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="1">
@@ -14887,38 +14887,38 @@
       <c r="B71" s="121">
         <v>0</v>
       </c>
-      <c r="C71" s="392">
-        <v>0</v>
-      </c>
-      <c r="D71" s="393">
+      <c r="C71" s="393">
+        <v>0</v>
+      </c>
+      <c r="D71" s="394">
         <f>IF(B76&gt;0,SUM(B71:B76)-C71,0)</f>
         <v>0</v>
       </c>
-      <c r="E71" s="392">
+      <c r="E71" s="393">
         <v>6.2</v>
       </c>
-      <c r="F71" s="392">
+      <c r="F71" s="393">
         <v>25.3</v>
       </c>
-      <c r="G71" s="394">
+      <c r="G71" s="395">
         <v>0</v>
       </c>
       <c r="H71" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I71" s="395">
+      <c r="I71" s="398">
         <f>IF($D$2&gt;F71,G71*($D$2-F71)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J71" s="395"/>
-      <c r="K71" s="395"/>
-      <c r="L71" s="395"/>
-      <c r="M71" s="395"/>
-      <c r="N71" s="395"/>
-      <c r="O71" s="395"/>
-      <c r="P71" s="395"/>
-      <c r="Q71" s="395"/>
+      <c r="J71" s="398"/>
+      <c r="K71" s="398"/>
+      <c r="L71" s="398"/>
+      <c r="M71" s="398"/>
+      <c r="N71" s="398"/>
+      <c r="O71" s="398"/>
+      <c r="P71" s="398"/>
+      <c r="Q71" s="398"/>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="1">
@@ -14927,24 +14927,24 @@
       <c r="B72" s="121">
         <v>0</v>
       </c>
-      <c r="C72" s="392"/>
-      <c r="D72" s="393"/>
-      <c r="E72" s="392"/>
-      <c r="F72" s="392"/>
-      <c r="G72" s="394"/>
+      <c r="C72" s="393"/>
+      <c r="D72" s="394"/>
+      <c r="E72" s="393"/>
+      <c r="F72" s="393"/>
+      <c r="G72" s="395"/>
       <c r="H72" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I72" s="395"/>
-      <c r="J72" s="395"/>
-      <c r="K72" s="395"/>
-      <c r="L72" s="395"/>
-      <c r="M72" s="395"/>
-      <c r="N72" s="395"/>
-      <c r="O72" s="395"/>
-      <c r="P72" s="395"/>
-      <c r="Q72" s="395"/>
+      <c r="I72" s="398"/>
+      <c r="J72" s="398"/>
+      <c r="K72" s="398"/>
+      <c r="L72" s="398"/>
+      <c r="M72" s="398"/>
+      <c r="N72" s="398"/>
+      <c r="O72" s="398"/>
+      <c r="P72" s="398"/>
+      <c r="Q72" s="398"/>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" s="1">
@@ -14953,24 +14953,24 @@
       <c r="B73" s="121">
         <v>0</v>
       </c>
-      <c r="C73" s="392"/>
-      <c r="D73" s="393"/>
-      <c r="E73" s="392"/>
-      <c r="F73" s="392"/>
-      <c r="G73" s="394"/>
+      <c r="C73" s="393"/>
+      <c r="D73" s="394"/>
+      <c r="E73" s="393"/>
+      <c r="F73" s="393"/>
+      <c r="G73" s="395"/>
       <c r="H73" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I73" s="395"/>
-      <c r="J73" s="395"/>
-      <c r="K73" s="395"/>
-      <c r="L73" s="395"/>
-      <c r="M73" s="395"/>
-      <c r="N73" s="395"/>
-      <c r="O73" s="395"/>
-      <c r="P73" s="395"/>
-      <c r="Q73" s="395"/>
+      <c r="I73" s="398"/>
+      <c r="J73" s="398"/>
+      <c r="K73" s="398"/>
+      <c r="L73" s="398"/>
+      <c r="M73" s="398"/>
+      <c r="N73" s="398"/>
+      <c r="O73" s="398"/>
+      <c r="P73" s="398"/>
+      <c r="Q73" s="398"/>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" s="1">
@@ -14979,24 +14979,24 @@
       <c r="B74" s="121">
         <v>0</v>
       </c>
-      <c r="C74" s="392"/>
-      <c r="D74" s="393"/>
-      <c r="E74" s="392"/>
-      <c r="F74" s="392"/>
-      <c r="G74" s="394"/>
+      <c r="C74" s="393"/>
+      <c r="D74" s="394"/>
+      <c r="E74" s="393"/>
+      <c r="F74" s="393"/>
+      <c r="G74" s="395"/>
       <c r="H74" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I74" s="395"/>
-      <c r="J74" s="395"/>
-      <c r="K74" s="395"/>
-      <c r="L74" s="395"/>
-      <c r="M74" s="395"/>
-      <c r="N74" s="395"/>
-      <c r="O74" s="395"/>
-      <c r="P74" s="395"/>
-      <c r="Q74" s="395"/>
+      <c r="I74" s="398"/>
+      <c r="J74" s="398"/>
+      <c r="K74" s="398"/>
+      <c r="L74" s="398"/>
+      <c r="M74" s="398"/>
+      <c r="N74" s="398"/>
+      <c r="O74" s="398"/>
+      <c r="P74" s="398"/>
+      <c r="Q74" s="398"/>
     </row>
     <row r="75" spans="1:17">
       <c r="A75" s="1">
@@ -15005,24 +15005,24 @@
       <c r="B75" s="121">
         <v>0</v>
       </c>
-      <c r="C75" s="392"/>
-      <c r="D75" s="393"/>
-      <c r="E75" s="392"/>
-      <c r="F75" s="392"/>
-      <c r="G75" s="394"/>
+      <c r="C75" s="393"/>
+      <c r="D75" s="394"/>
+      <c r="E75" s="393"/>
+      <c r="F75" s="393"/>
+      <c r="G75" s="395"/>
       <c r="H75" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I75" s="395"/>
-      <c r="J75" s="395"/>
-      <c r="K75" s="395"/>
-      <c r="L75" s="395"/>
-      <c r="M75" s="395"/>
-      <c r="N75" s="395"/>
-      <c r="O75" s="395"/>
-      <c r="P75" s="395"/>
-      <c r="Q75" s="395"/>
+      <c r="I75" s="398"/>
+      <c r="J75" s="398"/>
+      <c r="K75" s="398"/>
+      <c r="L75" s="398"/>
+      <c r="M75" s="398"/>
+      <c r="N75" s="398"/>
+      <c r="O75" s="398"/>
+      <c r="P75" s="398"/>
+      <c r="Q75" s="398"/>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" s="1">
@@ -15031,24 +15031,24 @@
       <c r="B76" s="121">
         <v>0</v>
       </c>
-      <c r="C76" s="392"/>
-      <c r="D76" s="393"/>
-      <c r="E76" s="392"/>
-      <c r="F76" s="392"/>
-      <c r="G76" s="394"/>
+      <c r="C76" s="393"/>
+      <c r="D76" s="394"/>
+      <c r="E76" s="393"/>
+      <c r="F76" s="393"/>
+      <c r="G76" s="395"/>
       <c r="H76" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I76" s="395"/>
-      <c r="J76" s="395"/>
-      <c r="K76" s="395"/>
-      <c r="L76" s="395"/>
-      <c r="M76" s="395"/>
-      <c r="N76" s="395"/>
-      <c r="O76" s="395"/>
-      <c r="P76" s="395"/>
-      <c r="Q76" s="395"/>
+      <c r="I76" s="398"/>
+      <c r="J76" s="398"/>
+      <c r="K76" s="398"/>
+      <c r="L76" s="398"/>
+      <c r="M76" s="398"/>
+      <c r="N76" s="398"/>
+      <c r="O76" s="398"/>
+      <c r="P76" s="398"/>
+      <c r="Q76" s="398"/>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" s="1">
@@ -15057,38 +15057,38 @@
       <c r="B77" s="121">
         <v>0</v>
       </c>
-      <c r="C77" s="392">
-        <v>0</v>
-      </c>
-      <c r="D77" s="393">
+      <c r="C77" s="393">
+        <v>0</v>
+      </c>
+      <c r="D77" s="394">
         <f>IF(B82&gt;0,SUM(B77:B82)-C77,0)</f>
         <v>0</v>
       </c>
-      <c r="E77" s="392">
+      <c r="E77" s="393">
         <v>6.2</v>
       </c>
-      <c r="F77" s="392">
+      <c r="F77" s="393">
         <v>25.3</v>
       </c>
-      <c r="G77" s="394">
+      <c r="G77" s="395">
         <v>0</v>
       </c>
       <c r="H77" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I77" s="395">
+      <c r="I77" s="398">
         <f>IF($D$2&gt;F77,G77*($D$2-F77)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J77" s="395"/>
-      <c r="K77" s="395"/>
-      <c r="L77" s="395"/>
-      <c r="M77" s="395"/>
-      <c r="N77" s="395"/>
-      <c r="O77" s="395"/>
-      <c r="P77" s="395"/>
-      <c r="Q77" s="395"/>
+      <c r="J77" s="398"/>
+      <c r="K77" s="398"/>
+      <c r="L77" s="398"/>
+      <c r="M77" s="398"/>
+      <c r="N77" s="398"/>
+      <c r="O77" s="398"/>
+      <c r="P77" s="398"/>
+      <c r="Q77" s="398"/>
     </row>
     <row r="78" spans="1:17">
       <c r="A78" s="1">
@@ -15097,24 +15097,24 @@
       <c r="B78" s="121">
         <v>0</v>
       </c>
-      <c r="C78" s="392"/>
-      <c r="D78" s="393"/>
-      <c r="E78" s="392"/>
-      <c r="F78" s="392"/>
-      <c r="G78" s="394"/>
+      <c r="C78" s="393"/>
+      <c r="D78" s="394"/>
+      <c r="E78" s="393"/>
+      <c r="F78" s="393"/>
+      <c r="G78" s="395"/>
       <c r="H78" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I78" s="395"/>
-      <c r="J78" s="395"/>
-      <c r="K78" s="395"/>
-      <c r="L78" s="395"/>
-      <c r="M78" s="395"/>
-      <c r="N78" s="395"/>
-      <c r="O78" s="395"/>
-      <c r="P78" s="395"/>
-      <c r="Q78" s="395"/>
+      <c r="I78" s="398"/>
+      <c r="J78" s="398"/>
+      <c r="K78" s="398"/>
+      <c r="L78" s="398"/>
+      <c r="M78" s="398"/>
+      <c r="N78" s="398"/>
+      <c r="O78" s="398"/>
+      <c r="P78" s="398"/>
+      <c r="Q78" s="398"/>
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="1">
@@ -15123,24 +15123,24 @@
       <c r="B79" s="121">
         <v>0</v>
       </c>
-      <c r="C79" s="392"/>
-      <c r="D79" s="393"/>
-      <c r="E79" s="392"/>
-      <c r="F79" s="392"/>
-      <c r="G79" s="394"/>
+      <c r="C79" s="393"/>
+      <c r="D79" s="394"/>
+      <c r="E79" s="393"/>
+      <c r="F79" s="393"/>
+      <c r="G79" s="395"/>
       <c r="H79" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I79" s="395"/>
-      <c r="J79" s="395"/>
-      <c r="K79" s="395"/>
-      <c r="L79" s="395"/>
-      <c r="M79" s="395"/>
-      <c r="N79" s="395"/>
-      <c r="O79" s="395"/>
-      <c r="P79" s="395"/>
-      <c r="Q79" s="395"/>
+      <c r="I79" s="398"/>
+      <c r="J79" s="398"/>
+      <c r="K79" s="398"/>
+      <c r="L79" s="398"/>
+      <c r="M79" s="398"/>
+      <c r="N79" s="398"/>
+      <c r="O79" s="398"/>
+      <c r="P79" s="398"/>
+      <c r="Q79" s="398"/>
     </row>
     <row r="80" spans="1:17">
       <c r="A80" s="1">
@@ -15149,24 +15149,24 @@
       <c r="B80" s="121">
         <v>0</v>
       </c>
-      <c r="C80" s="392"/>
-      <c r="D80" s="393"/>
-      <c r="E80" s="392"/>
-      <c r="F80" s="392"/>
-      <c r="G80" s="394"/>
+      <c r="C80" s="393"/>
+      <c r="D80" s="394"/>
+      <c r="E80" s="393"/>
+      <c r="F80" s="393"/>
+      <c r="G80" s="395"/>
       <c r="H80" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I80" s="395"/>
-      <c r="J80" s="395"/>
-      <c r="K80" s="395"/>
-      <c r="L80" s="395"/>
-      <c r="M80" s="395"/>
-      <c r="N80" s="395"/>
-      <c r="O80" s="395"/>
-      <c r="P80" s="395"/>
-      <c r="Q80" s="395"/>
+      <c r="I80" s="398"/>
+      <c r="J80" s="398"/>
+      <c r="K80" s="398"/>
+      <c r="L80" s="398"/>
+      <c r="M80" s="398"/>
+      <c r="N80" s="398"/>
+      <c r="O80" s="398"/>
+      <c r="P80" s="398"/>
+      <c r="Q80" s="398"/>
     </row>
     <row r="81" spans="1:17">
       <c r="A81" s="1">
@@ -15175,24 +15175,24 @@
       <c r="B81" s="121">
         <v>0</v>
       </c>
-      <c r="C81" s="392"/>
-      <c r="D81" s="393"/>
-      <c r="E81" s="392"/>
-      <c r="F81" s="392"/>
-      <c r="G81" s="394"/>
+      <c r="C81" s="393"/>
+      <c r="D81" s="394"/>
+      <c r="E81" s="393"/>
+      <c r="F81" s="393"/>
+      <c r="G81" s="395"/>
       <c r="H81" s="120">
         <f t="shared" ref="H81:H88" si="3">R87*0.25</f>
         <v>0</v>
       </c>
-      <c r="I81" s="395"/>
-      <c r="J81" s="395"/>
-      <c r="K81" s="395"/>
-      <c r="L81" s="395"/>
-      <c r="M81" s="395"/>
-      <c r="N81" s="395"/>
-      <c r="O81" s="395"/>
-      <c r="P81" s="395"/>
-      <c r="Q81" s="395"/>
+      <c r="I81" s="398"/>
+      <c r="J81" s="398"/>
+      <c r="K81" s="398"/>
+      <c r="L81" s="398"/>
+      <c r="M81" s="398"/>
+      <c r="N81" s="398"/>
+      <c r="O81" s="398"/>
+      <c r="P81" s="398"/>
+      <c r="Q81" s="398"/>
     </row>
     <row r="82" spans="1:17">
       <c r="A82" s="1">
@@ -15201,24 +15201,24 @@
       <c r="B82" s="121">
         <v>0</v>
       </c>
-      <c r="C82" s="392"/>
-      <c r="D82" s="393"/>
-      <c r="E82" s="392"/>
-      <c r="F82" s="392"/>
-      <c r="G82" s="394"/>
+      <c r="C82" s="393"/>
+      <c r="D82" s="394"/>
+      <c r="E82" s="393"/>
+      <c r="F82" s="393"/>
+      <c r="G82" s="395"/>
       <c r="H82" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I82" s="395"/>
-      <c r="J82" s="395"/>
-      <c r="K82" s="395"/>
-      <c r="L82" s="395"/>
-      <c r="M82" s="395"/>
-      <c r="N82" s="395"/>
-      <c r="O82" s="395"/>
-      <c r="P82" s="395"/>
-      <c r="Q82" s="395"/>
+      <c r="I82" s="398"/>
+      <c r="J82" s="398"/>
+      <c r="K82" s="398"/>
+      <c r="L82" s="398"/>
+      <c r="M82" s="398"/>
+      <c r="N82" s="398"/>
+      <c r="O82" s="398"/>
+      <c r="P82" s="398"/>
+      <c r="Q82" s="398"/>
     </row>
     <row r="83" spans="1:17">
       <c r="A83" s="1">
@@ -15227,38 +15227,38 @@
       <c r="B83" s="121">
         <v>0</v>
       </c>
-      <c r="C83" s="392">
-        <v>0</v>
-      </c>
-      <c r="D83" s="393">
+      <c r="C83" s="393">
+        <v>0</v>
+      </c>
+      <c r="D83" s="394">
         <f>IF(B88&gt;0,SUM(B83:B88)-C83,0)</f>
         <v>0</v>
       </c>
-      <c r="E83" s="392">
+      <c r="E83" s="393">
         <v>6.2</v>
       </c>
-      <c r="F83" s="392">
+      <c r="F83" s="393">
         <v>25.3</v>
       </c>
-      <c r="G83" s="394">
+      <c r="G83" s="395">
         <v>0</v>
       </c>
       <c r="H83" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I83" s="395">
+      <c r="I83" s="398">
         <f>IF($D$2&gt;F83,G83*($D$2-F83)*0.2,0)</f>
         <v>0</v>
       </c>
-      <c r="J83" s="395"/>
-      <c r="K83" s="395"/>
-      <c r="L83" s="395"/>
-      <c r="M83" s="395"/>
-      <c r="N83" s="395"/>
-      <c r="O83" s="395"/>
-      <c r="P83" s="395"/>
-      <c r="Q83" s="395"/>
+      <c r="J83" s="398"/>
+      <c r="K83" s="398"/>
+      <c r="L83" s="398"/>
+      <c r="M83" s="398"/>
+      <c r="N83" s="398"/>
+      <c r="O83" s="398"/>
+      <c r="P83" s="398"/>
+      <c r="Q83" s="398"/>
     </row>
     <row r="84" spans="1:17">
       <c r="A84" s="1">
@@ -15267,24 +15267,24 @@
       <c r="B84" s="121">
         <v>0</v>
       </c>
-      <c r="C84" s="392"/>
-      <c r="D84" s="393"/>
-      <c r="E84" s="392"/>
-      <c r="F84" s="392"/>
-      <c r="G84" s="394"/>
+      <c r="C84" s="393"/>
+      <c r="D84" s="394"/>
+      <c r="E84" s="393"/>
+      <c r="F84" s="393"/>
+      <c r="G84" s="395"/>
       <c r="H84" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I84" s="395"/>
-      <c r="J84" s="395"/>
-      <c r="K84" s="395"/>
-      <c r="L84" s="395"/>
-      <c r="M84" s="395"/>
-      <c r="N84" s="395"/>
-      <c r="O84" s="395"/>
-      <c r="P84" s="395"/>
-      <c r="Q84" s="395"/>
+      <c r="I84" s="398"/>
+      <c r="J84" s="398"/>
+      <c r="K84" s="398"/>
+      <c r="L84" s="398"/>
+      <c r="M84" s="398"/>
+      <c r="N84" s="398"/>
+      <c r="O84" s="398"/>
+      <c r="P84" s="398"/>
+      <c r="Q84" s="398"/>
     </row>
     <row r="85" spans="1:17">
       <c r="A85" s="1">
@@ -15293,24 +15293,24 @@
       <c r="B85" s="121">
         <v>0</v>
       </c>
-      <c r="C85" s="392"/>
-      <c r="D85" s="393"/>
-      <c r="E85" s="392"/>
-      <c r="F85" s="392"/>
-      <c r="G85" s="394"/>
+      <c r="C85" s="393"/>
+      <c r="D85" s="394"/>
+      <c r="E85" s="393"/>
+      <c r="F85" s="393"/>
+      <c r="G85" s="395"/>
       <c r="H85" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I85" s="395"/>
-      <c r="J85" s="395"/>
-      <c r="K85" s="395"/>
-      <c r="L85" s="395"/>
-      <c r="M85" s="395"/>
-      <c r="N85" s="395"/>
-      <c r="O85" s="395"/>
-      <c r="P85" s="395"/>
-      <c r="Q85" s="395"/>
+      <c r="I85" s="398"/>
+      <c r="J85" s="398"/>
+      <c r="K85" s="398"/>
+      <c r="L85" s="398"/>
+      <c r="M85" s="398"/>
+      <c r="N85" s="398"/>
+      <c r="O85" s="398"/>
+      <c r="P85" s="398"/>
+      <c r="Q85" s="398"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" s="1">
@@ -15319,24 +15319,24 @@
       <c r="B86" s="121">
         <v>0</v>
       </c>
-      <c r="C86" s="392"/>
-      <c r="D86" s="393"/>
-      <c r="E86" s="392"/>
-      <c r="F86" s="392"/>
-      <c r="G86" s="394"/>
+      <c r="C86" s="393"/>
+      <c r="D86" s="394"/>
+      <c r="E86" s="393"/>
+      <c r="F86" s="393"/>
+      <c r="G86" s="395"/>
       <c r="H86" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I86" s="395"/>
-      <c r="J86" s="395"/>
-      <c r="K86" s="395"/>
-      <c r="L86" s="395"/>
-      <c r="M86" s="395"/>
-      <c r="N86" s="395"/>
-      <c r="O86" s="395"/>
-      <c r="P86" s="395"/>
-      <c r="Q86" s="395"/>
+      <c r="I86" s="398"/>
+      <c r="J86" s="398"/>
+      <c r="K86" s="398"/>
+      <c r="L86" s="398"/>
+      <c r="M86" s="398"/>
+      <c r="N86" s="398"/>
+      <c r="O86" s="398"/>
+      <c r="P86" s="398"/>
+      <c r="Q86" s="398"/>
     </row>
     <row r="87" spans="1:17">
       <c r="A87" s="1">
@@ -15345,24 +15345,24 @@
       <c r="B87" s="121">
         <v>0</v>
       </c>
-      <c r="C87" s="392"/>
-      <c r="D87" s="393"/>
-      <c r="E87" s="392"/>
-      <c r="F87" s="392"/>
-      <c r="G87" s="394"/>
+      <c r="C87" s="393"/>
+      <c r="D87" s="394"/>
+      <c r="E87" s="393"/>
+      <c r="F87" s="393"/>
+      <c r="G87" s="395"/>
       <c r="H87" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I87" s="395"/>
-      <c r="J87" s="395"/>
-      <c r="K87" s="395"/>
-      <c r="L87" s="395"/>
-      <c r="M87" s="395"/>
-      <c r="N87" s="395"/>
-      <c r="O87" s="395"/>
-      <c r="P87" s="395"/>
-      <c r="Q87" s="395"/>
+      <c r="I87" s="398"/>
+      <c r="J87" s="398"/>
+      <c r="K87" s="398"/>
+      <c r="L87" s="398"/>
+      <c r="M87" s="398"/>
+      <c r="N87" s="398"/>
+      <c r="O87" s="398"/>
+      <c r="P87" s="398"/>
+      <c r="Q87" s="398"/>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" s="1">
@@ -15371,94 +15371,125 @@
       <c r="B88" s="121">
         <v>0</v>
       </c>
-      <c r="C88" s="392"/>
-      <c r="D88" s="393"/>
-      <c r="E88" s="392"/>
-      <c r="F88" s="392"/>
-      <c r="G88" s="394"/>
+      <c r="C88" s="393"/>
+      <c r="D88" s="394"/>
+      <c r="E88" s="393"/>
+      <c r="F88" s="393"/>
+      <c r="G88" s="395"/>
       <c r="H88" s="120">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I88" s="395"/>
-      <c r="J88" s="395"/>
-      <c r="K88" s="395"/>
-      <c r="L88" s="395"/>
-      <c r="M88" s="395"/>
-      <c r="N88" s="395"/>
-      <c r="O88" s="395"/>
-      <c r="P88" s="395"/>
-      <c r="Q88" s="395"/>
+      <c r="I88" s="398"/>
+      <c r="J88" s="398"/>
+      <c r="K88" s="398"/>
+      <c r="L88" s="398"/>
+      <c r="M88" s="398"/>
+      <c r="N88" s="398"/>
+      <c r="O88" s="398"/>
+      <c r="P88" s="398"/>
+      <c r="Q88" s="398"/>
     </row>
   </sheetData>
   <mergeCells count="189">
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="E10:E15"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="O10:O15"/>
-    <mergeCell ref="P10:P15"/>
-    <mergeCell ref="Q10:Q15"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="D16:D21"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="F16:F21"/>
-    <mergeCell ref="G16:G21"/>
-    <mergeCell ref="I16:I21"/>
-    <mergeCell ref="J16:J21"/>
-    <mergeCell ref="I10:I15"/>
-    <mergeCell ref="J10:J15"/>
-    <mergeCell ref="K10:K15"/>
-    <mergeCell ref="L10:L15"/>
-    <mergeCell ref="M10:M15"/>
-    <mergeCell ref="N10:N15"/>
-    <mergeCell ref="Q16:Q21"/>
-    <mergeCell ref="K16:K21"/>
-    <mergeCell ref="L16:L21"/>
-    <mergeCell ref="M16:M21"/>
-    <mergeCell ref="N16:N21"/>
-    <mergeCell ref="O16:O21"/>
-    <mergeCell ref="P16:P21"/>
-    <mergeCell ref="P22:P27"/>
-    <mergeCell ref="Q22:Q27"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="D28:D34"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="F28:F34"/>
-    <mergeCell ref="G28:G34"/>
-    <mergeCell ref="O28:O34"/>
-    <mergeCell ref="P28:P34"/>
-    <mergeCell ref="Q28:Q34"/>
-    <mergeCell ref="K28:K34"/>
-    <mergeCell ref="L28:L34"/>
-    <mergeCell ref="M28:M34"/>
-    <mergeCell ref="N28:N34"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="F22:F27"/>
-    <mergeCell ref="G22:G27"/>
-    <mergeCell ref="I22:I27"/>
-    <mergeCell ref="J22:J27"/>
-    <mergeCell ref="K22:K27"/>
-    <mergeCell ref="L22:L27"/>
-    <mergeCell ref="F35:F40"/>
-    <mergeCell ref="G35:G40"/>
-    <mergeCell ref="I35:I40"/>
-    <mergeCell ref="J35:J40"/>
-    <mergeCell ref="I28:I34"/>
-    <mergeCell ref="J28:J34"/>
-    <mergeCell ref="M22:M27"/>
-    <mergeCell ref="N22:N27"/>
-    <mergeCell ref="O22:O27"/>
+    <mergeCell ref="C83:C88"/>
+    <mergeCell ref="D83:D88"/>
+    <mergeCell ref="E83:E88"/>
+    <mergeCell ref="F83:F88"/>
+    <mergeCell ref="G83:G88"/>
+    <mergeCell ref="O83:O88"/>
+    <mergeCell ref="P83:P88"/>
+    <mergeCell ref="Q83:Q88"/>
+    <mergeCell ref="I83:I88"/>
+    <mergeCell ref="J83:J88"/>
+    <mergeCell ref="K83:K88"/>
+    <mergeCell ref="L83:L88"/>
+    <mergeCell ref="M83:M88"/>
+    <mergeCell ref="N83:N88"/>
+    <mergeCell ref="M71:M76"/>
+    <mergeCell ref="N71:N76"/>
+    <mergeCell ref="O71:O76"/>
+    <mergeCell ref="P71:P76"/>
+    <mergeCell ref="M77:M82"/>
+    <mergeCell ref="N77:N82"/>
+    <mergeCell ref="O77:O82"/>
+    <mergeCell ref="P77:P82"/>
+    <mergeCell ref="Q77:Q82"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="D77:D82"/>
+    <mergeCell ref="E77:E82"/>
+    <mergeCell ref="F77:F82"/>
+    <mergeCell ref="G77:G82"/>
+    <mergeCell ref="I77:I82"/>
+    <mergeCell ref="J77:J82"/>
+    <mergeCell ref="K77:K82"/>
+    <mergeCell ref="L77:L82"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="G65:G70"/>
+    <mergeCell ref="O65:O70"/>
+    <mergeCell ref="P65:P70"/>
+    <mergeCell ref="Q65:Q70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="D71:D76"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="F71:F76"/>
+    <mergeCell ref="G71:G76"/>
+    <mergeCell ref="I71:I76"/>
+    <mergeCell ref="J71:J76"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="J65:J70"/>
+    <mergeCell ref="K65:K70"/>
+    <mergeCell ref="L65:L70"/>
+    <mergeCell ref="M65:M70"/>
+    <mergeCell ref="N65:N70"/>
+    <mergeCell ref="Q71:Q76"/>
+    <mergeCell ref="K71:K76"/>
+    <mergeCell ref="L71:L76"/>
+    <mergeCell ref="M53:M58"/>
+    <mergeCell ref="N53:N58"/>
+    <mergeCell ref="O53:O58"/>
+    <mergeCell ref="P53:P58"/>
+    <mergeCell ref="M59:M64"/>
+    <mergeCell ref="N59:N64"/>
+    <mergeCell ref="O59:O64"/>
+    <mergeCell ref="P59:P64"/>
+    <mergeCell ref="Q59:Q64"/>
+    <mergeCell ref="C59:C64"/>
+    <mergeCell ref="D59:D64"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="F59:F64"/>
+    <mergeCell ref="G59:G64"/>
+    <mergeCell ref="I59:I64"/>
+    <mergeCell ref="J59:J64"/>
+    <mergeCell ref="K59:K64"/>
+    <mergeCell ref="L59:L64"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="F47:F52"/>
+    <mergeCell ref="G47:G52"/>
+    <mergeCell ref="O47:O52"/>
+    <mergeCell ref="P47:P52"/>
+    <mergeCell ref="Q47:Q52"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="D53:D58"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="F53:F58"/>
+    <mergeCell ref="G53:G58"/>
+    <mergeCell ref="I53:I58"/>
+    <mergeCell ref="J53:J58"/>
+    <mergeCell ref="I47:I52"/>
+    <mergeCell ref="J47:J52"/>
+    <mergeCell ref="K47:K52"/>
+    <mergeCell ref="L47:L52"/>
+    <mergeCell ref="M47:M52"/>
+    <mergeCell ref="N47:N52"/>
+    <mergeCell ref="Q53:Q58"/>
+    <mergeCell ref="K53:K58"/>
+    <mergeCell ref="L53:L58"/>
     <mergeCell ref="Q35:Q40"/>
     <mergeCell ref="C41:C46"/>
     <mergeCell ref="D41:D46"/>
@@ -15483,104 +15514,73 @@
     <mergeCell ref="C35:C40"/>
     <mergeCell ref="D35:D40"/>
     <mergeCell ref="E35:E40"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="F47:F52"/>
-    <mergeCell ref="G47:G52"/>
-    <mergeCell ref="O47:O52"/>
-    <mergeCell ref="P47:P52"/>
-    <mergeCell ref="Q47:Q52"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="F53:F58"/>
-    <mergeCell ref="G53:G58"/>
-    <mergeCell ref="I53:I58"/>
-    <mergeCell ref="J53:J58"/>
-    <mergeCell ref="I47:I52"/>
-    <mergeCell ref="J47:J52"/>
-    <mergeCell ref="K47:K52"/>
-    <mergeCell ref="L47:L52"/>
-    <mergeCell ref="M47:M52"/>
-    <mergeCell ref="N47:N52"/>
-    <mergeCell ref="Q53:Q58"/>
-    <mergeCell ref="K53:K58"/>
-    <mergeCell ref="L53:L58"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="D59:D64"/>
-    <mergeCell ref="E59:E64"/>
-    <mergeCell ref="F59:F64"/>
-    <mergeCell ref="G59:G64"/>
-    <mergeCell ref="I59:I64"/>
-    <mergeCell ref="J59:J64"/>
-    <mergeCell ref="K59:K64"/>
-    <mergeCell ref="L59:L64"/>
-    <mergeCell ref="M53:M58"/>
-    <mergeCell ref="N53:N58"/>
-    <mergeCell ref="O53:O58"/>
-    <mergeCell ref="P53:P58"/>
-    <mergeCell ref="M59:M64"/>
-    <mergeCell ref="N59:N64"/>
-    <mergeCell ref="O59:O64"/>
-    <mergeCell ref="P59:P64"/>
-    <mergeCell ref="Q59:Q64"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="G65:G70"/>
-    <mergeCell ref="O65:O70"/>
-    <mergeCell ref="P65:P70"/>
-    <mergeCell ref="Q65:Q70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="D71:D76"/>
-    <mergeCell ref="E71:E76"/>
-    <mergeCell ref="F71:F76"/>
-    <mergeCell ref="G71:G76"/>
-    <mergeCell ref="I71:I76"/>
-    <mergeCell ref="J71:J76"/>
-    <mergeCell ref="I65:I70"/>
-    <mergeCell ref="J65:J70"/>
-    <mergeCell ref="K65:K70"/>
-    <mergeCell ref="L65:L70"/>
-    <mergeCell ref="M65:M70"/>
-    <mergeCell ref="N65:N70"/>
-    <mergeCell ref="Q71:Q76"/>
-    <mergeCell ref="K71:K76"/>
-    <mergeCell ref="L71:L76"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="D77:D82"/>
-    <mergeCell ref="E77:E82"/>
-    <mergeCell ref="F77:F82"/>
-    <mergeCell ref="G77:G82"/>
-    <mergeCell ref="I77:I82"/>
-    <mergeCell ref="J77:J82"/>
-    <mergeCell ref="K77:K82"/>
-    <mergeCell ref="L77:L82"/>
-    <mergeCell ref="M71:M76"/>
-    <mergeCell ref="N71:N76"/>
-    <mergeCell ref="O71:O76"/>
-    <mergeCell ref="P71:P76"/>
-    <mergeCell ref="M77:M82"/>
-    <mergeCell ref="N77:N82"/>
-    <mergeCell ref="O77:O82"/>
-    <mergeCell ref="P77:P82"/>
-    <mergeCell ref="Q77:Q82"/>
-    <mergeCell ref="C83:C88"/>
-    <mergeCell ref="D83:D88"/>
-    <mergeCell ref="E83:E88"/>
-    <mergeCell ref="F83:F88"/>
-    <mergeCell ref="G83:G88"/>
-    <mergeCell ref="O83:O88"/>
-    <mergeCell ref="P83:P88"/>
-    <mergeCell ref="Q83:Q88"/>
-    <mergeCell ref="I83:I88"/>
-    <mergeCell ref="J83:J88"/>
-    <mergeCell ref="K83:K88"/>
-    <mergeCell ref="L83:L88"/>
-    <mergeCell ref="M83:M88"/>
-    <mergeCell ref="N83:N88"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="I35:I40"/>
+    <mergeCell ref="J35:J40"/>
+    <mergeCell ref="I28:I34"/>
+    <mergeCell ref="J28:J34"/>
+    <mergeCell ref="M22:M27"/>
+    <mergeCell ref="N22:N27"/>
+    <mergeCell ref="O22:O27"/>
+    <mergeCell ref="P22:P27"/>
+    <mergeCell ref="Q22:Q27"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="D28:D34"/>
+    <mergeCell ref="E28:E34"/>
+    <mergeCell ref="F28:F34"/>
+    <mergeCell ref="G28:G34"/>
+    <mergeCell ref="O28:O34"/>
+    <mergeCell ref="P28:P34"/>
+    <mergeCell ref="Q28:Q34"/>
+    <mergeCell ref="K28:K34"/>
+    <mergeCell ref="L28:L34"/>
+    <mergeCell ref="M28:M34"/>
+    <mergeCell ref="N28:N34"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="G22:G27"/>
+    <mergeCell ref="I22:I27"/>
+    <mergeCell ref="J22:J27"/>
+    <mergeCell ref="K22:K27"/>
+    <mergeCell ref="L22:L27"/>
+    <mergeCell ref="O10:O15"/>
+    <mergeCell ref="P10:P15"/>
+    <mergeCell ref="Q10:Q15"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="G16:G21"/>
+    <mergeCell ref="I16:I21"/>
+    <mergeCell ref="J16:J21"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="K10:K15"/>
+    <mergeCell ref="L10:L15"/>
+    <mergeCell ref="M10:M15"/>
+    <mergeCell ref="N10:N15"/>
+    <mergeCell ref="Q16:Q21"/>
+    <mergeCell ref="K16:K21"/>
+    <mergeCell ref="L16:L21"/>
+    <mergeCell ref="M16:M21"/>
+    <mergeCell ref="N16:N21"/>
+    <mergeCell ref="O16:O21"/>
+    <mergeCell ref="P16:P21"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17013,29 +17013,29 @@
     </row>
     <row r="6" spans="4:12" ht="17.100000000000001" customHeight="1">
       <c r="F6" s="245"/>
-      <c r="G6" s="459" t="s">
+      <c r="G6" s="467" t="s">
         <v>1283</v>
       </c>
-      <c r="H6" s="461" t="s">
+      <c r="H6" s="469" t="s">
         <v>1284</v>
       </c>
-      <c r="I6" s="461" t="s">
+      <c r="I6" s="469" t="s">
         <v>1285</v>
       </c>
-      <c r="J6" s="461" t="s">
+      <c r="J6" s="469" t="s">
         <v>1286</v>
       </c>
-      <c r="K6" s="450" t="s">
+      <c r="K6" s="465" t="s">
         <v>1287</v>
       </c>
-      <c r="L6" s="451"/>
+      <c r="L6" s="466"/>
     </row>
     <row r="7" spans="4:12" ht="18" customHeight="1">
       <c r="F7" s="245"/>
-      <c r="G7" s="460"/>
-      <c r="H7" s="462"/>
-      <c r="I7" s="462"/>
-      <c r="J7" s="462"/>
+      <c r="G7" s="468"/>
+      <c r="H7" s="470"/>
+      <c r="I7" s="470"/>
+      <c r="J7" s="470"/>
       <c r="K7" s="246" t="s">
         <v>1288</v>
       </c>
@@ -17044,11 +17044,11 @@
       </c>
     </row>
     <row r="8" spans="4:12" ht="30" customHeight="1" thickBot="1">
-      <c r="D8" s="458" t="s">
+      <c r="D8" s="456" t="s">
         <v>1290</v>
       </c>
-      <c r="E8" s="458"/>
-      <c r="F8" s="458"/>
+      <c r="E8" s="456"/>
+      <c r="F8" s="456"/>
       <c r="G8" s="248">
         <v>9.6</v>
       </c>
@@ -17094,21 +17094,21 @@
     </row>
     <row r="12" spans="4:12" ht="18.75">
       <c r="F12" s="245"/>
-      <c r="G12" s="452" t="s">
+      <c r="G12" s="450" t="s">
         <v>1291</v>
       </c>
-      <c r="H12" s="454" t="s">
+      <c r="H12" s="452" t="s">
         <v>1292</v>
       </c>
-      <c r="I12" s="456" t="s">
+      <c r="I12" s="454" t="s">
         <v>1293</v>
       </c>
-      <c r="J12" s="457"/>
+      <c r="J12" s="455"/>
     </row>
     <row r="13" spans="4:12" ht="18.75">
       <c r="F13" s="245"/>
-      <c r="G13" s="453"/>
-      <c r="H13" s="455"/>
+      <c r="G13" s="451"/>
+      <c r="H13" s="453"/>
       <c r="I13" s="251" t="s">
         <v>1294</v>
       </c>
@@ -17117,11 +17117,11 @@
       </c>
     </row>
     <row r="14" spans="4:12" ht="33" customHeight="1" thickBot="1">
-      <c r="D14" s="458" t="s">
+      <c r="D14" s="456" t="s">
         <v>1296</v>
       </c>
-      <c r="E14" s="458"/>
-      <c r="F14" s="458"/>
+      <c r="E14" s="456"/>
+      <c r="F14" s="456"/>
       <c r="G14" s="253" t="s">
         <v>1297</v>
       </c>
@@ -17139,20 +17139,20 @@
     </row>
     <row r="16" spans="4:12" ht="15.75" thickBot="1"/>
     <row r="17" spans="4:10" ht="18.75">
-      <c r="G17" s="452" t="s">
+      <c r="G17" s="450" t="s">
         <v>1298</v>
       </c>
-      <c r="H17" s="454" t="s">
+      <c r="H17" s="452" t="s">
         <v>1292</v>
       </c>
-      <c r="I17" s="456" t="s">
+      <c r="I17" s="454" t="s">
         <v>1293</v>
       </c>
-      <c r="J17" s="457"/>
+      <c r="J17" s="455"/>
     </row>
     <row r="18" spans="4:10" ht="18.75">
-      <c r="G18" s="453"/>
-      <c r="H18" s="455"/>
+      <c r="G18" s="451"/>
+      <c r="H18" s="453"/>
       <c r="I18" s="251" t="s">
         <v>1294</v>
       </c>
@@ -17161,11 +17161,11 @@
       </c>
     </row>
     <row r="19" spans="4:10" ht="33" customHeight="1" thickBot="1">
-      <c r="D19" s="458" t="s">
+      <c r="D19" s="456" t="s">
         <v>1296</v>
       </c>
-      <c r="E19" s="458"/>
-      <c r="F19" s="458"/>
+      <c r="E19" s="456"/>
+      <c r="F19" s="456"/>
       <c r="G19" s="253" t="s">
         <v>1299</v>
       </c>
@@ -17183,20 +17183,20 @@
     </row>
     <row r="21" spans="4:10" ht="15.75" thickBot="1"/>
     <row r="22" spans="4:10" ht="18.75">
-      <c r="G22" s="463" t="s">
+      <c r="G22" s="457" t="s">
         <v>1300</v>
       </c>
-      <c r="H22" s="454" t="s">
+      <c r="H22" s="452" t="s">
         <v>1292</v>
       </c>
-      <c r="I22" s="456" t="s">
+      <c r="I22" s="454" t="s">
         <v>1293</v>
       </c>
-      <c r="J22" s="457"/>
+      <c r="J22" s="455"/>
     </row>
     <row r="23" spans="4:10" ht="18.75">
-      <c r="G23" s="464"/>
-      <c r="H23" s="455"/>
+      <c r="G23" s="458"/>
+      <c r="H23" s="453"/>
       <c r="I23" s="251" t="s">
         <v>1294</v>
       </c>
@@ -17205,11 +17205,11 @@
       </c>
     </row>
     <row r="24" spans="4:10" ht="32.1" customHeight="1">
-      <c r="D24" s="458" t="s">
+      <c r="D24" s="456" t="s">
         <v>1296</v>
       </c>
-      <c r="E24" s="458"/>
-      <c r="F24" s="458"/>
+      <c r="E24" s="456"/>
+      <c r="F24" s="456"/>
       <c r="G24" s="254" t="s">
         <v>1301</v>
       </c>
@@ -17264,20 +17264,20 @@
     </row>
     <row r="29" spans="4:10" ht="15.75" thickBot="1"/>
     <row r="30" spans="4:10" ht="18.75">
-      <c r="G30" s="465" t="s">
+      <c r="G30" s="459" t="s">
         <v>1304</v>
       </c>
-      <c r="H30" s="467" t="s">
+      <c r="H30" s="461" t="s">
         <v>1305</v>
       </c>
-      <c r="I30" s="469" t="s">
+      <c r="I30" s="463" t="s">
         <v>1306</v>
       </c>
-      <c r="J30" s="470"/>
+      <c r="J30" s="464"/>
     </row>
     <row r="31" spans="4:10" ht="18.75">
-      <c r="G31" s="466"/>
-      <c r="H31" s="468"/>
+      <c r="G31" s="460"/>
+      <c r="H31" s="462"/>
       <c r="I31" s="258" t="s">
         <v>1288</v>
       </c>
@@ -17286,11 +17286,11 @@
       </c>
     </row>
     <row r="32" spans="4:10" ht="35.1" customHeight="1" thickBot="1">
-      <c r="D32" s="458" t="s">
+      <c r="D32" s="456" t="s">
         <v>1307</v>
       </c>
-      <c r="E32" s="458"/>
-      <c r="F32" s="458"/>
+      <c r="E32" s="456"/>
+      <c r="F32" s="456"/>
       <c r="G32" s="260" t="s">
         <v>1301</v>
       </c>
@@ -17308,6 +17308,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:J17"/>
@@ -17320,16 +17330,6 @@
     <mergeCell ref="G30:G31"/>
     <mergeCell ref="H30:H31"/>
     <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19078,17 +19078,17 @@
   <sheetData>
     <row r="1" spans="1:40" ht="17.25" thickBot="1">
       <c r="A1" s="304"/>
-      <c r="B1" s="437" t="s">
+      <c r="B1" s="404" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="438"/>
-      <c r="D1" s="438"/>
-      <c r="E1" s="438"/>
-      <c r="F1" s="439"/>
-      <c r="G1" s="440" t="s">
+      <c r="C1" s="405"/>
+      <c r="D1" s="405"/>
+      <c r="E1" s="405"/>
+      <c r="F1" s="406"/>
+      <c r="G1" s="407" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="441"/>
+      <c r="H1" s="408"/>
     </row>
     <row r="2" spans="1:40" ht="17.25" thickBot="1">
       <c r="A2" s="307" t="s">
@@ -19109,11 +19109,11 @@
       <c r="F2" s="309" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="442">
+      <c r="G2" s="409">
         <f ca="1">TODAY()-A13</f>
         <v>1116</v>
       </c>
-      <c r="H2" s="443"/>
+      <c r="H2" s="410"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
       <c r="A3" s="310">
@@ -19140,10 +19140,10 @@
         <f>'whobor-touna'!L3</f>
         <v>20849.739999999998</v>
       </c>
-      <c r="G3" s="440" t="s">
+      <c r="G3" s="407" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="441"/>
+      <c r="H3" s="408"/>
     </row>
     <row r="4" spans="1:40" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="315"/>
@@ -19164,11 +19164,11 @@
         <f>F3/$B$3</f>
         <v>1.5308597043787142E-2</v>
       </c>
-      <c r="G4" s="435">
+      <c r="G4" s="411">
         <f ca="1">A6/G2</f>
         <v>201.68989141577043</v>
       </c>
-      <c r="H4" s="436"/>
+      <c r="H4" s="412"/>
     </row>
     <row r="5" spans="1:40" ht="17.25" thickBot="1">
       <c r="A5" s="318" t="s">
@@ -19189,10 +19189,10 @@
       <c r="F5" s="322" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="432" t="s">
+      <c r="G5" s="418" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="433"/>
+      <c r="H5" s="419"/>
     </row>
     <row r="6" spans="1:40" ht="15.75" customHeight="1" thickBot="1">
       <c r="A6" s="323">
@@ -19219,205 +19219,205 @@
         <f>D6-E6</f>
         <v>1822693.9888200001</v>
       </c>
-      <c r="G6" s="435">
+      <c r="G6" s="411">
         <f ca="1">G4*30</f>
         <v>6050.6967424731129</v>
       </c>
-      <c r="H6" s="436"/>
+      <c r="H6" s="412"/>
     </row>
     <row r="7" spans="1:40" s="330" customFormat="1" ht="20.25">
       <c r="A7" s="329"/>
-      <c r="B7" s="429" t="s">
+      <c r="B7" s="431" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="427"/>
-      <c r="D7" s="427"/>
-      <c r="E7" s="428"/>
-      <c r="F7" s="430"/>
-      <c r="G7" s="426" t="s">
+      <c r="C7" s="429"/>
+      <c r="D7" s="429"/>
+      <c r="E7" s="430"/>
+      <c r="F7" s="432"/>
+      <c r="G7" s="428" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="427"/>
-      <c r="I7" s="427"/>
-      <c r="J7" s="428"/>
-      <c r="K7" s="428"/>
-      <c r="L7" s="420" t="s">
+      <c r="H7" s="429"/>
+      <c r="I7" s="429"/>
+      <c r="J7" s="430"/>
+      <c r="K7" s="430"/>
+      <c r="L7" s="424" t="s">
         <v>1275</v>
       </c>
-      <c r="M7" s="421"/>
-      <c r="N7" s="421"/>
-      <c r="O7" s="421"/>
-      <c r="P7" s="421"/>
-      <c r="Q7" s="422"/>
-      <c r="R7" s="421" t="s">
+      <c r="M7" s="420"/>
+      <c r="N7" s="420"/>
+      <c r="O7" s="420"/>
+      <c r="P7" s="420"/>
+      <c r="Q7" s="425"/>
+      <c r="R7" s="420" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="421"/>
-      <c r="T7" s="421"/>
-      <c r="U7" s="421"/>
-      <c r="V7" s="421"/>
-      <c r="W7" s="421"/>
-      <c r="X7" s="420" t="s">
+      <c r="S7" s="420"/>
+      <c r="T7" s="420"/>
+      <c r="U7" s="420"/>
+      <c r="V7" s="420"/>
+      <c r="W7" s="420"/>
+      <c r="X7" s="424" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="421"/>
-      <c r="Z7" s="421"/>
-      <c r="AA7" s="421"/>
-      <c r="AB7" s="421"/>
-      <c r="AC7" s="422"/>
+      <c r="Y7" s="420"/>
+      <c r="Z7" s="420"/>
+      <c r="AA7" s="420"/>
+      <c r="AB7" s="420"/>
+      <c r="AC7" s="425"/>
     </row>
     <row r="8" spans="1:40" s="330" customFormat="1" ht="16.5">
       <c r="A8" s="331" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="423" t="s">
+      <c r="B8" s="426" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="424"/>
-      <c r="D8" s="424"/>
-      <c r="E8" s="424"/>
-      <c r="F8" s="425"/>
-      <c r="G8" s="424" t="s">
+      <c r="C8" s="421"/>
+      <c r="D8" s="421"/>
+      <c r="E8" s="421"/>
+      <c r="F8" s="427"/>
+      <c r="G8" s="421" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="424"/>
-      <c r="I8" s="424"/>
-      <c r="J8" s="424"/>
-      <c r="K8" s="424"/>
-      <c r="L8" s="423" t="s">
+      <c r="H8" s="421"/>
+      <c r="I8" s="421"/>
+      <c r="J8" s="421"/>
+      <c r="K8" s="421"/>
+      <c r="L8" s="426" t="s">
         <v>1276</v>
       </c>
-      <c r="M8" s="424"/>
-      <c r="N8" s="424"/>
-      <c r="O8" s="424"/>
-      <c r="P8" s="424"/>
-      <c r="Q8" s="425"/>
-      <c r="R8" s="424" t="s">
+      <c r="M8" s="421"/>
+      <c r="N8" s="421"/>
+      <c r="O8" s="421"/>
+      <c r="P8" s="421"/>
+      <c r="Q8" s="427"/>
+      <c r="R8" s="421" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="424"/>
-      <c r="T8" s="424"/>
-      <c r="U8" s="424"/>
-      <c r="V8" s="424"/>
-      <c r="W8" s="424"/>
-      <c r="X8" s="423" t="s">
+      <c r="S8" s="421"/>
+      <c r="T8" s="421"/>
+      <c r="U8" s="421"/>
+      <c r="V8" s="421"/>
+      <c r="W8" s="421"/>
+      <c r="X8" s="426" t="s">
         <v>196</v>
       </c>
-      <c r="Y8" s="424"/>
-      <c r="Z8" s="424"/>
-      <c r="AA8" s="424"/>
-      <c r="AB8" s="424"/>
-      <c r="AC8" s="425"/>
+      <c r="Y8" s="421"/>
+      <c r="Z8" s="421"/>
+      <c r="AA8" s="421"/>
+      <c r="AB8" s="421"/>
+      <c r="AC8" s="427"/>
       <c r="AK8" s="332"/>
     </row>
     <row r="9" spans="1:40" s="330" customFormat="1" ht="16.5">
       <c r="A9" s="331" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="408" t="s">
+      <c r="B9" s="415" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="409"/>
-      <c r="D9" s="408" t="s">
+      <c r="C9" s="414"/>
+      <c r="D9" s="415" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="413"/>
-      <c r="F9" s="419"/>
-      <c r="G9" s="431" t="s">
+      <c r="E9" s="416"/>
+      <c r="F9" s="443"/>
+      <c r="G9" s="413" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="409"/>
-      <c r="I9" s="408" t="s">
+      <c r="H9" s="414"/>
+      <c r="I9" s="415" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="413"/>
-      <c r="K9" s="412"/>
-      <c r="L9" s="406" t="s">
+      <c r="J9" s="416"/>
+      <c r="K9" s="417"/>
+      <c r="L9" s="435" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="407"/>
-      <c r="N9" s="412" t="s">
+      <c r="M9" s="423"/>
+      <c r="N9" s="417" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="413"/>
-      <c r="P9" s="413"/>
-      <c r="Q9" s="414"/>
-      <c r="R9" s="434" t="s">
+      <c r="O9" s="416"/>
+      <c r="P9" s="416"/>
+      <c r="Q9" s="438"/>
+      <c r="R9" s="422" t="s">
         <v>30</v>
       </c>
-      <c r="S9" s="407"/>
-      <c r="T9" s="412" t="s">
+      <c r="S9" s="423"/>
+      <c r="T9" s="417" t="s">
         <v>47</v>
       </c>
-      <c r="U9" s="413"/>
-      <c r="V9" s="413"/>
-      <c r="W9" s="413"/>
-      <c r="X9" s="406" t="s">
+      <c r="U9" s="416"/>
+      <c r="V9" s="416"/>
+      <c r="W9" s="416"/>
+      <c r="X9" s="435" t="s">
         <v>49</v>
       </c>
-      <c r="Y9" s="407"/>
-      <c r="Z9" s="412" t="s">
+      <c r="Y9" s="423"/>
+      <c r="Z9" s="417" t="s">
         <v>50</v>
       </c>
-      <c r="AA9" s="413"/>
-      <c r="AB9" s="413"/>
-      <c r="AC9" s="414"/>
+      <c r="AA9" s="416"/>
+      <c r="AB9" s="416"/>
+      <c r="AC9" s="438"/>
     </row>
     <row r="10" spans="1:40" ht="15.75" customHeight="1">
       <c r="A10" s="333" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="404" t="s">
+      <c r="B10" s="433" t="s">
         <v>283</v>
       </c>
-      <c r="C10" s="405"/>
-      <c r="D10" s="416">
+      <c r="C10" s="434"/>
+      <c r="D10" s="440">
         <f>'whobor-touna'!G3/$B$3</f>
         <v>0.3861106502158409</v>
       </c>
-      <c r="E10" s="410"/>
-      <c r="F10" s="411"/>
-      <c r="G10" s="415" t="s">
+      <c r="E10" s="436"/>
+      <c r="F10" s="437"/>
+      <c r="G10" s="439" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="405"/>
-      <c r="I10" s="416">
+      <c r="H10" s="434"/>
+      <c r="I10" s="440">
         <f>'thmei-touna'!G3/$B$3</f>
         <v>0.55258928433890697</v>
       </c>
-      <c r="J10" s="410"/>
-      <c r="K10" s="410"/>
-      <c r="L10" s="417" t="s">
+      <c r="J10" s="436"/>
+      <c r="K10" s="436"/>
+      <c r="L10" s="441" t="s">
         <v>283</v>
       </c>
-      <c r="M10" s="418"/>
-      <c r="N10" s="410">
+      <c r="M10" s="442"/>
+      <c r="N10" s="436">
         <f>宜人贷!T2/$B$3</f>
         <v>0</v>
       </c>
-      <c r="O10" s="410"/>
-      <c r="P10" s="410"/>
-      <c r="Q10" s="411"/>
-      <c r="R10" s="418"/>
-      <c r="S10" s="418"/>
-      <c r="T10" s="410">
+      <c r="O10" s="436"/>
+      <c r="P10" s="436"/>
+      <c r="Q10" s="437"/>
+      <c r="R10" s="442"/>
+      <c r="S10" s="442"/>
+      <c r="T10" s="436">
         <f>宜人贷!Z2/$B$3</f>
         <v>0</v>
       </c>
-      <c r="U10" s="410"/>
-      <c r="V10" s="410"/>
-      <c r="W10" s="410"/>
-      <c r="X10" s="417">
+      <c r="U10" s="436"/>
+      <c r="V10" s="436"/>
+      <c r="W10" s="436"/>
+      <c r="X10" s="441">
         <v>830106</v>
       </c>
-      <c r="Y10" s="418"/>
-      <c r="Z10" s="410">
+      <c r="Y10" s="442"/>
+      <c r="Z10" s="436">
         <f>'whobor-wzd'!L2/$B$3</f>
         <v>3.9235681925590307E-2</v>
       </c>
-      <c r="AA10" s="410"/>
-      <c r="AB10" s="410"/>
-      <c r="AC10" s="411"/>
+      <c r="AA10" s="436"/>
+      <c r="AB10" s="436"/>
+      <c r="AC10" s="437"/>
     </row>
     <row r="11" spans="1:40" ht="28.5" customHeight="1">
       <c r="A11" s="334" t="s">
@@ -36257,27 +36257,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="R8:W8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="X7:AC7"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="L8:Q8"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="L7:Q7"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="B9:C9"/>
@@ -36294,6 +36273,27 @@
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D9:F9"/>
+    <mergeCell ref="X7:AC7"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="R8:W8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36307,8 +36307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -42646,7 +42646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P396"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>

</xml_diff>